<commit_message>
Latest changes in UAT2 environment  suites
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="5580" windowWidth="16215" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="4290" windowWidth="13755" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="5"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="469">
   <si>
     <t>Ankit</t>
   </si>
@@ -1327,27 +1327,6 @@
     <t>s9650899231111111</t>
   </si>
   <si>
-    <t>sdxdfzs@gmail.com</t>
-  </si>
-  <si>
-    <t>fcr@gmail.com</t>
-  </si>
-  <si>
-    <t>cdfv@gmail.com</t>
-  </si>
-  <si>
-    <t>fcdgv@gmail.com</t>
-  </si>
-  <si>
-    <t>svfd@gmail.com</t>
-  </si>
-  <si>
-    <t>vcfdv@gmail.com</t>
-  </si>
-  <si>
-    <t>vcv@gmail.com</t>
-  </si>
-  <si>
     <t>s96508992311111111</t>
   </si>
   <si>
@@ -1426,7 +1405,25 @@
     <t>SS_CheckOut_GuestUser_EmptyField</t>
   </si>
   <si>
-    <t>SS_ItemDelete_OneItem_CheckOut</t>
+    <t>fcaqr@gmail.com</t>
+  </si>
+  <si>
+    <t>sdxdss@gmail.com</t>
+  </si>
+  <si>
+    <t>fcdZAgv@gmail.com</t>
+  </si>
+  <si>
+    <t>ssavfd@gmail.com</t>
+  </si>
+  <si>
+    <t>vcfsxcfdv@gmail.com</t>
+  </si>
+  <si>
+    <t>vcvdzsw@gmail.com</t>
+  </si>
+  <si>
+    <t>cdAzsZSfv@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2050,13 +2047,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CH284"/>
+  <dimension ref="A1:CH283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="CV143" xSplit="1" ySplit="1"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="BB137" xSplit="1" ySplit="1"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="CY153" pane="bottomRight" sqref="CY153"/>
+      <selection activeCell="BD147" pane="bottomRight" sqref="BD147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4485,7 +4482,7 @@
         <v>365</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>438</v>
+        <v>468</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -6361,7 +6358,7 @@
       <c r="CE43" s="1"/>
       <c r="CF43" s="18"/>
       <c r="CG43" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="1:85" x14ac:dyDescent="0.25">
@@ -7453,7 +7450,7 @@
     </row>
     <row r="55" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>365</v>
@@ -7466,7 +7463,7 @@
         <v>53</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -8167,7 +8164,7 @@
       <c r="CE61" s="1"/>
       <c r="CF61" s="18"/>
       <c r="CG61" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="62" spans="1:85" x14ac:dyDescent="0.25">
@@ -9896,7 +9893,7 @@
       <c r="AS79" s="1"/>
       <c r="AT79" s="1"/>
       <c r="AU79" s="27" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="AV79" s="1"/>
       <c r="AW79" s="1"/>
@@ -16164,7 +16161,7 @@
       <c r="B136" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" s="26" t="s">
         <v>429</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -16284,9 +16281,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="137" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="137" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>365</v>
@@ -16411,9 +16408,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="138" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="138" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>406</v>
+        <v>428</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>365</v>
@@ -16538,9 +16535,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="139" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="139" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>365</v>
@@ -16665,18 +16662,18 @@
         <v>366</v>
       </c>
     </row>
-    <row r="140" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="140" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>429</v>
+      <c r="C140" s="26" t="s">
+        <v>409</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>362</v>
+        <v>3</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -16792,9 +16789,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="141" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="141" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>365</v>
@@ -16811,7 +16808,7 @@
         <v>53</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>325</v>
+        <v>416</v>
       </c>
       <c r="I141" s="1"/>
       <c r="J141" s="2" t="s">
@@ -16919,15 +16916,15 @@
         <v>366</v>
       </c>
     </row>
-    <row r="142" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="142" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C142" s="26" t="s">
-        <v>409</v>
+      <c r="C142" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>3</v>
@@ -16938,7 +16935,7 @@
         <v>53</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>416</v>
+        <v>325</v>
       </c>
       <c r="I142" s="1"/>
       <c r="J142" s="2" t="s">
@@ -17046,9 +17043,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="143" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="143" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>365</v>
@@ -17173,9 +17170,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="144" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="144" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>399</v>
+        <v>134</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>365</v>
@@ -17237,12 +17234,8 @@
       <c r="AK144" s="1"/>
       <c r="AL144" s="1"/>
       <c r="AM144" s="1"/>
-      <c r="AN144" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="AO144" s="1" t="s">
-        <v>397</v>
-      </c>
+      <c r="AN144" s="1"/>
+      <c r="AO144" s="1"/>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
       <c r="AR144" s="1"/>
@@ -17255,30 +17248,30 @@
       <c r="AY144" s="1"/>
       <c r="AZ144" s="1"/>
       <c r="BA144" s="1" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="BB144" s="1"/>
       <c r="BC144" s="1"/>
       <c r="BD144" s="1"/>
       <c r="BE144" s="1"/>
-      <c r="BF144" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG144" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="BH144" s="1"/>
-      <c r="BI144" s="1"/>
-      <c r="BJ144" s="1"/>
-      <c r="BK144" s="1"/>
-      <c r="BL144" s="1" t="s">
-        <v>430</v>
-      </c>
+      <c r="BF144" s="1"/>
+      <c r="BG144" s="1"/>
+      <c r="BH144" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BI144" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ144" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BK144" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="BL144" s="1"/>
       <c r="BM144" s="1"/>
       <c r="BN144" s="1"/>
-      <c r="BO144" s="1" t="s">
-        <v>400</v>
-      </c>
+      <c r="BO144" s="1"/>
       <c r="BP144" s="1"/>
       <c r="BQ144" s="1"/>
       <c r="BR144" s="1"/>
@@ -17300,18 +17293,18 @@
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="145" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>134</v>
+        <v>337</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>3</v>
+      <c r="C145" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="D145" s="26" t="s">
+        <v>362</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -17387,16 +17380,16 @@
       <c r="BF145" s="1"/>
       <c r="BG145" s="1"/>
       <c r="BH145" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="BI145" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BJ145" s="1" t="s">
-        <v>330</v>
+        <v>141</v>
+      </c>
+      <c r="BI145" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="BJ145" t="s">
+        <v>341</v>
       </c>
       <c r="BK145" s="1" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="BL145" s="1"/>
       <c r="BM145" s="1"/>
@@ -17410,32 +17403,38 @@
       <c r="BU145" s="1"/>
       <c r="BV145" s="1"/>
       <c r="BW145" s="1"/>
-      <c r="BX145" s="1"/>
-      <c r="BY145" s="1"/>
-      <c r="BZ145" s="1"/>
-      <c r="CA145" s="1"/>
+      <c r="BX145" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BY145" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="BZ145" t="s">
+        <v>343</v>
+      </c>
+      <c r="CA145" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="CB145" s="1"/>
       <c r="CC145" s="1"/>
       <c r="CD145" s="1"/>
       <c r="CE145" s="1"/>
       <c r="CF145" s="1"/>
       <c r="CG145" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="146" spans="1:85" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row customFormat="1" r="146" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>337</v>
+        <v>461</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C146" s="26" t="s">
-        <v>381</v>
-      </c>
-      <c r="D146" s="26" t="s">
-        <v>362</v>
-      </c>
+      <c r="C146" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="2" t="s">
@@ -17501,26 +17500,22 @@
       <c r="AY146" s="1"/>
       <c r="AZ146" s="1"/>
       <c r="BA146" s="1" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="BB146" s="1"/>
       <c r="BC146" s="1"/>
       <c r="BD146" s="1"/>
       <c r="BE146" s="1"/>
-      <c r="BF146" s="1"/>
-      <c r="BG146" s="1"/>
-      <c r="BH146" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BI146" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="BJ146" t="s">
-        <v>341</v>
-      </c>
-      <c r="BK146" s="1" t="s">
-        <v>342</v>
-      </c>
+      <c r="BF146" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BG146" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BH146" s="1"/>
+      <c r="BI146" s="1"/>
+      <c r="BJ146" s="1"/>
+      <c r="BK146" s="1"/>
       <c r="BL146" s="1"/>
       <c r="BM146" s="1"/>
       <c r="BN146" s="1"/>
@@ -17533,38 +17528,32 @@
       <c r="BU146" s="1"/>
       <c r="BV146" s="1"/>
       <c r="BW146" s="1"/>
-      <c r="BX146" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BY146" s="17" t="s">
-        <v>340</v>
-      </c>
-      <c r="BZ146" t="s">
-        <v>343</v>
-      </c>
-      <c r="CA146" s="1" t="s">
-        <v>344</v>
-      </c>
+      <c r="BX146" s="1"/>
+      <c r="BY146" s="1"/>
+      <c r="BZ146" s="1"/>
+      <c r="CA146" s="1"/>
       <c r="CB146" s="1"/>
       <c r="CC146" s="1"/>
       <c r="CD146" s="1"/>
       <c r="CE146" s="1"/>
       <c r="CF146" s="1"/>
       <c r="CG146" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="147" spans="1:85" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row customFormat="1" r="147" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>468</v>
+        <v>136</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D147" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
       <c r="G147" s="2" t="s">
@@ -17630,18 +17619,21 @@
       <c r="AY147" s="1"/>
       <c r="AZ147" s="1"/>
       <c r="BA147" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BB147" s="1"/>
-      <c r="BC147" s="1"/>
-      <c r="BD147" s="1"/>
-      <c r="BE147" s="1"/>
-      <c r="BF147" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG147" s="4" t="s">
-        <v>132</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="BB147" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD147" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE147" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF147" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG147" s="1"/>
       <c r="BH147" s="1"/>
       <c r="BI147" s="1"/>
       <c r="BJ147" s="1"/>
@@ -17671,9 +17663,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="148" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="148" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>365</v>
@@ -17749,21 +17741,18 @@
       <c r="AY148" s="1"/>
       <c r="AZ148" s="1"/>
       <c r="BA148" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BB148" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD148" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE148" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF148" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="BG148" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="BB148" s="1"/>
+      <c r="BC148" s="1"/>
+      <c r="BD148" s="1"/>
+      <c r="BE148" s="1"/>
+      <c r="BF148" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BG148" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="BH148" s="1"/>
       <c r="BI148" s="1"/>
       <c r="BJ148" s="1"/>
@@ -17793,9 +17782,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="149" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="149" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>365</v>
@@ -17870,23 +17859,25 @@
       <c r="AX149" s="1"/>
       <c r="AY149" s="1"/>
       <c r="AZ149" s="1"/>
-      <c r="BA149" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="BA149" s="1"/>
       <c r="BB149" s="1"/>
       <c r="BC149" s="1"/>
       <c r="BD149" s="1"/>
       <c r="BE149" s="1"/>
-      <c r="BF149" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG149" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="BH149" s="1"/>
-      <c r="BI149" s="1"/>
-      <c r="BJ149" s="1"/>
-      <c r="BK149" s="1"/>
+      <c r="BF149" s="1"/>
+      <c r="BG149" s="1"/>
+      <c r="BH149" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BI149" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ149" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BK149" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="BL149" s="1"/>
       <c r="BM149" s="1"/>
       <c r="BN149" s="1"/>
@@ -17912,19 +17903,17 @@
         <v>366</v>
       </c>
     </row>
-    <row r="150" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="150" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="2" t="s">
@@ -17989,25 +17978,26 @@
       <c r="AX150" s="1"/>
       <c r="AY150" s="1"/>
       <c r="AZ150" s="1"/>
-      <c r="BA150" s="1"/>
-      <c r="BB150" s="1"/>
-      <c r="BC150" s="1"/>
-      <c r="BD150" s="1"/>
-      <c r="BE150" s="1"/>
-      <c r="BF150" s="1"/>
+      <c r="BA150" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB150" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD150" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE150" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF150" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="BG150" s="1"/>
-      <c r="BH150" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BI150" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BJ150" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="BK150" s="1" t="s">
-        <v>331</v>
-      </c>
+      <c r="BH150" s="1"/>
+      <c r="BI150" s="1"/>
+      <c r="BJ150" s="1"/>
+      <c r="BK150" s="1"/>
       <c r="BL150" s="1"/>
       <c r="BM150" s="1"/>
       <c r="BN150" s="1"/>
@@ -18033,9 +18023,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="151" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="151" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>365</v>
@@ -18109,21 +18099,18 @@
       <c r="AY151" s="1"/>
       <c r="AZ151" s="1"/>
       <c r="BA151" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BB151" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD151" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE151" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF151" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="BG151" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="BB151" s="1"/>
+      <c r="BC151" s="1"/>
+      <c r="BD151" s="1"/>
+      <c r="BE151" s="1"/>
+      <c r="BF151" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BG151" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="BH151" s="1"/>
       <c r="BI151" s="1"/>
       <c r="BJ151" s="1"/>
@@ -18155,15 +18142,17 @@
     </row>
     <row customFormat="1" r="152" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>143</v>
+        <v>392</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D152" s="1"/>
+      <c r="C152" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
       <c r="G152" s="2" t="s">
@@ -18248,7 +18237,9 @@
       <c r="BL152" s="1"/>
       <c r="BM152" s="1"/>
       <c r="BN152" s="1"/>
-      <c r="BO152" s="1"/>
+      <c r="BO152" s="1" t="s">
+        <v>400</v>
+      </c>
       <c r="BP152" s="1"/>
       <c r="BQ152" s="1"/>
       <c r="BR152" s="1"/>
@@ -18267,27 +18258,29 @@
       <c r="CE152" s="1"/>
       <c r="CF152" s="1"/>
       <c r="CG152" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row customFormat="1" r="153" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>469</v>
+        <v>402</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C153" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D153" s="1"/>
+      <c r="C153" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="2" t="s">
         <v>53</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>467</v>
+        <v>325</v>
       </c>
       <c r="I153" s="1"/>
       <c r="J153" s="2" t="s">
@@ -18345,21 +18338,31 @@
       <c r="AX153" s="1"/>
       <c r="AY153" s="1"/>
       <c r="AZ153" s="1"/>
-      <c r="BA153" s="1"/>
+      <c r="BA153" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BB153" s="1"/>
       <c r="BC153" s="1"/>
       <c r="BD153" s="1"/>
       <c r="BE153" s="1"/>
-      <c r="BF153" s="1"/>
-      <c r="BG153" s="4"/>
+      <c r="BF153" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BG153" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="BH153" s="1"/>
       <c r="BI153" s="1"/>
       <c r="BJ153" s="1"/>
       <c r="BK153" s="1"/>
-      <c r="BL153" s="1"/>
+      <c r="BL153" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="BM153" s="1"/>
       <c r="BN153" s="1"/>
-      <c r="BO153" s="1"/>
+      <c r="BO153" s="1" t="s">
+        <v>400</v>
+      </c>
       <c r="BP153" s="1"/>
       <c r="BQ153" s="1"/>
       <c r="BR153" s="1"/>
@@ -18383,7 +18386,7 @@
     </row>
     <row customFormat="1" r="154" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>365</v>
@@ -18475,12 +18478,12 @@
       <c r="BI154" s="1"/>
       <c r="BJ154" s="1"/>
       <c r="BK154" s="1"/>
-      <c r="BL154" s="1"/>
+      <c r="BL154" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="BM154" s="1"/>
       <c r="BN154" s="1"/>
-      <c r="BO154" s="1" t="s">
-        <v>400</v>
-      </c>
+      <c r="BO154" s="1"/>
       <c r="BP154" s="1"/>
       <c r="BQ154" s="1"/>
       <c r="BR154" s="1"/>
@@ -18504,17 +18507,15 @@
     </row>
     <row customFormat="1" r="155" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>402</v>
+        <v>144</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C155" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C155" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D155" s="1"/>
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
       <c r="G155" s="2" t="s">
@@ -18579,31 +18580,29 @@
       <c r="AX155" s="1"/>
       <c r="AY155" s="1"/>
       <c r="AZ155" s="1"/>
-      <c r="BA155" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="BA155" s="1"/>
       <c r="BB155" s="1"/>
       <c r="BC155" s="1"/>
       <c r="BD155" s="1"/>
       <c r="BE155" s="1"/>
-      <c r="BF155" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG155" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="BH155" s="1"/>
-      <c r="BI155" s="1"/>
-      <c r="BJ155" s="1"/>
-      <c r="BK155" s="1"/>
-      <c r="BL155" s="1" t="s">
-        <v>430</v>
-      </c>
+      <c r="BF155" s="1"/>
+      <c r="BG155" s="1"/>
+      <c r="BH155" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BI155" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ155" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BK155" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="BL155" s="1"/>
       <c r="BM155" s="1"/>
       <c r="BN155" s="1"/>
-      <c r="BO155" s="1" t="s">
-        <v>400</v>
-      </c>
+      <c r="BO155" s="1"/>
       <c r="BP155" s="1"/>
       <c r="BQ155" s="1"/>
       <c r="BR155" s="1"/>
@@ -18627,19 +18626,21 @@
     </row>
     <row customFormat="1" r="156" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>403</v>
+        <v>145</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>393</v>
+        <v>464</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
+      <c r="F156" t="s">
+        <v>3</v>
+      </c>
       <c r="G156" s="2" t="s">
         <v>53</v>
       </c>
@@ -18671,7 +18672,9 @@
       <c r="S156" s="1"/>
       <c r="T156" s="1"/>
       <c r="U156" s="1"/>
-      <c r="V156" s="1"/>
+      <c r="V156" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="W156" s="1"/>
       <c r="X156" s="1"/>
       <c r="Y156" s="1"/>
@@ -18682,13 +18685,19 @@
       <c r="AD156" s="1"/>
       <c r="AE156" s="1"/>
       <c r="AF156" s="1"/>
-      <c r="AG156" s="1"/>
+      <c r="AG156" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AH156" s="1"/>
-      <c r="AI156" s="1"/>
+      <c r="AI156" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AJ156" s="1"/>
       <c r="AK156" s="1"/>
       <c r="AL156" s="1"/>
-      <c r="AM156" s="1"/>
+      <c r="AM156" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AN156" s="1"/>
       <c r="AO156" s="1"/>
       <c r="AP156" s="1"/>
@@ -18703,25 +18712,26 @@
       <c r="AY156" s="1"/>
       <c r="AZ156" s="1"/>
       <c r="BA156" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BB156" s="1"/>
-      <c r="BC156" s="1"/>
-      <c r="BD156" s="1"/>
-      <c r="BE156" s="1"/>
-      <c r="BF156" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG156" s="4" t="s">
-        <v>132</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="BB156" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD156" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE156" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF156" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BG156" s="1"/>
       <c r="BH156" s="1"/>
       <c r="BI156" s="1"/>
       <c r="BJ156" s="1"/>
       <c r="BK156" s="1"/>
-      <c r="BL156" s="1" t="s">
-        <v>430</v>
-      </c>
+      <c r="BL156" s="1"/>
       <c r="BM156" s="1"/>
       <c r="BN156" s="1"/>
       <c r="BO156" s="1"/>
@@ -18743,22 +18753,26 @@
       <c r="CE156" s="1"/>
       <c r="CF156" s="1"/>
       <c r="CG156" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row customFormat="1" r="157" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D157" s="1"/>
+      <c r="C157" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
+      <c r="F157" t="s">
+        <v>3</v>
+      </c>
       <c r="G157" s="2" t="s">
         <v>53</v>
       </c>
@@ -18790,7 +18804,9 @@
       <c r="S157" s="1"/>
       <c r="T157" s="1"/>
       <c r="U157" s="1"/>
-      <c r="V157" s="1"/>
+      <c r="V157" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="W157" s="1"/>
       <c r="X157" s="1"/>
       <c r="Y157" s="1"/>
@@ -18801,13 +18817,19 @@
       <c r="AD157" s="1"/>
       <c r="AE157" s="1"/>
       <c r="AF157" s="1"/>
-      <c r="AG157" s="1"/>
+      <c r="AG157" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AH157" s="1"/>
-      <c r="AI157" s="1"/>
+      <c r="AI157" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AJ157" s="1"/>
       <c r="AK157" s="1"/>
       <c r="AL157" s="1"/>
-      <c r="AM157" s="1"/>
+      <c r="AM157" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AN157" s="1"/>
       <c r="AO157" s="1"/>
       <c r="AP157" s="1"/>
@@ -18821,25 +18843,23 @@
       <c r="AX157" s="1"/>
       <c r="AY157" s="1"/>
       <c r="AZ157" s="1"/>
-      <c r="BA157" s="1"/>
+      <c r="BA157" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BB157" s="1"/>
       <c r="BC157" s="1"/>
       <c r="BD157" s="1"/>
       <c r="BE157" s="1"/>
-      <c r="BF157" s="1"/>
-      <c r="BG157" s="1"/>
-      <c r="BH157" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BI157" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BJ157" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="BK157" s="1" t="s">
-        <v>331</v>
-      </c>
+      <c r="BF157" t="s">
+        <v>148</v>
+      </c>
+      <c r="BG157" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="BH157" s="1"/>
+      <c r="BI157" s="1"/>
+      <c r="BJ157" s="1"/>
+      <c r="BK157" s="1"/>
       <c r="BL157" s="1"/>
       <c r="BM157" s="1"/>
       <c r="BN157" s="1"/>
@@ -18867,13 +18887,13 @@
     </row>
     <row customFormat="1" r="158" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>439</v>
+        <v>466</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>3</v>
@@ -18952,26 +18972,25 @@
       <c r="AX158" s="1"/>
       <c r="AY158" s="1"/>
       <c r="AZ158" s="1"/>
-      <c r="BA158" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BB158" s="4" t="s">
+      <c r="BA158" s="1"/>
+      <c r="BB158" s="1"/>
+      <c r="BC158" s="1"/>
+      <c r="BD158" s="1"/>
+      <c r="BE158" s="1"/>
+      <c r="BF158" s="1"/>
+      <c r="BG158" s="1"/>
+      <c r="BH158" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BI158" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="BD158" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE158" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF158" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BG158" s="1"/>
-      <c r="BH158" s="1"/>
-      <c r="BI158" s="1"/>
-      <c r="BJ158" s="1"/>
-      <c r="BK158" s="1"/>
+      <c r="BJ158" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BK158" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="BL158" s="1"/>
       <c r="BM158" s="1"/>
       <c r="BN158" s="1"/>
@@ -18999,13 +19018,13 @@
     </row>
     <row customFormat="1" r="159" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>146</v>
+        <v>312</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C159" s="26" t="s">
-        <v>440</v>
+        <v>467</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>3</v>
@@ -19084,19 +19103,12 @@
       <c r="AX159" s="1"/>
       <c r="AY159" s="1"/>
       <c r="AZ159" s="1"/>
-      <c r="BA159" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BB159" s="1"/>
-      <c r="BC159" s="1"/>
-      <c r="BD159" s="1"/>
-      <c r="BE159" s="1"/>
-      <c r="BF159" t="s">
-        <v>148</v>
-      </c>
-      <c r="BG159" s="4" t="s">
-        <v>147</v>
-      </c>
+      <c r="BA159" s="1"/>
+      <c r="BB159" s="4"/>
+      <c r="BD159" s="2"/>
+      <c r="BE159" s="3"/>
+      <c r="BF159" s="2"/>
+      <c r="BG159" s="1"/>
       <c r="BH159" s="1"/>
       <c r="BI159" s="1"/>
       <c r="BJ159" s="1"/>
@@ -19127,56 +19139,32 @@
       </c>
     </row>
     <row customFormat="1" r="160" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>149</v>
+      <c r="A160" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C160" s="26" t="s">
-        <v>441</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
       <c r="E160" s="1"/>
-      <c r="F160" t="s">
-        <v>3</v>
-      </c>
-      <c r="G160" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H160" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
       <c r="I160" s="1"/>
-      <c r="J160" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K160" t="s">
-        <v>1</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M160" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N160" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
       <c r="O160" s="1"/>
-      <c r="P160" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="P160" s="1"/>
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
       <c r="S160" s="1"/>
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
-      <c r="V160" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="V160" s="1"/>
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
       <c r="Y160" s="1"/>
@@ -19187,19 +19175,13 @@
       <c r="AD160" s="1"/>
       <c r="AE160" s="1"/>
       <c r="AF160" s="1"/>
-      <c r="AG160" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="AG160" s="1"/>
       <c r="AH160" s="1"/>
-      <c r="AI160" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="AI160" s="1"/>
       <c r="AJ160" s="1"/>
       <c r="AK160" s="1"/>
       <c r="AL160" s="1"/>
-      <c r="AM160" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="AM160" s="1"/>
       <c r="AN160" s="1"/>
       <c r="AO160" s="1"/>
       <c r="AP160" s="1"/>
@@ -19220,18 +19202,10 @@
       <c r="BE160" s="1"/>
       <c r="BF160" s="1"/>
       <c r="BG160" s="1"/>
-      <c r="BH160" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="BI160" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BJ160" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="BK160" s="1" t="s">
-        <v>331</v>
-      </c>
+      <c r="BH160" s="1"/>
+      <c r="BI160" s="11"/>
+      <c r="BJ160" s="1"/>
+      <c r="BK160" s="1"/>
       <c r="BL160" s="1"/>
       <c r="BM160" s="1"/>
       <c r="BN160" s="1"/>
@@ -19253,42 +19227,40 @@
       <c r="CD160" s="1"/>
       <c r="CE160" s="1"/>
       <c r="CF160" s="1"/>
-      <c r="CG160" t="s">
-        <v>366</v>
-      </c>
+      <c r="CG160" s="1"/>
     </row>
     <row customFormat="1" r="161" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>312</v>
+        <v>248</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C161" s="26" t="s">
-        <v>442</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E161" s="1"/>
-      <c r="F161" t="s">
-        <v>3</v>
-      </c>
-      <c r="G161" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H161" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="I161" s="1"/>
-      <c r="J161" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K161" t="s">
-        <v>1</v>
+      <c r="C161" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="D161" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I161" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="J161" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="K161" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="L161" s="1" t="s">
-        <v>5</v>
+        <v>350</v>
       </c>
       <c r="M161" s="2" t="s">
         <v>28</v>
@@ -19300,14 +19272,22 @@
       <c r="P161" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q161" s="1"/>
-      <c r="R161" s="1"/>
-      <c r="S161" s="1"/>
-      <c r="T161" s="1"/>
-      <c r="U161" s="1"/>
-      <c r="V161" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="Q161" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="R161" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="S161" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="T161" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="U161" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="V161" s="1"/>
       <c r="W161" s="1"/>
       <c r="X161" s="1"/>
       <c r="Y161" s="1"/>
@@ -19319,18 +19299,14 @@
       <c r="AE161" s="1"/>
       <c r="AF161" s="1"/>
       <c r="AG161" s="1" t="s">
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="AH161" s="1"/>
-      <c r="AI161" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="AI161" s="1"/>
       <c r="AJ161" s="1"/>
       <c r="AK161" s="1"/>
       <c r="AL161" s="1"/>
-      <c r="AM161" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="AM161" s="1"/>
       <c r="AN161" s="1"/>
       <c r="AO161" s="1"/>
       <c r="AP161" s="1"/>
@@ -19344,14 +19320,24 @@
       <c r="AX161" s="1"/>
       <c r="AY161" s="1"/>
       <c r="AZ161" s="1"/>
-      <c r="BA161" s="1"/>
-      <c r="BB161" s="4"/>
-      <c r="BD161" s="2"/>
-      <c r="BE161" s="3"/>
-      <c r="BF161" s="2"/>
+      <c r="BA161" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB161" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD161" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE161" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF161" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="BG161" s="1"/>
       <c r="BH161" s="1"/>
-      <c r="BI161" s="1"/>
+      <c r="BI161" s="11"/>
       <c r="BJ161" s="1"/>
       <c r="BK161" s="1"/>
       <c r="BL161" s="1"/>
@@ -19374,37 +19360,69 @@
       <c r="CC161" s="1"/>
       <c r="CD161" s="1"/>
       <c r="CE161" s="1"/>
-      <c r="CF161" s="1"/>
+      <c r="CF161" s="18"/>
       <c r="CG161" t="s">
         <v>366</v>
       </c>
     </row>
     <row customFormat="1" r="162" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A162" s="9" t="s">
-        <v>240</v>
+      <c r="A162" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
-      <c r="F162" s="1"/>
-      <c r="G162" s="1"/>
-      <c r="H162" s="1"/>
-      <c r="I162" s="1"/>
-      <c r="J162" s="1"/>
-      <c r="K162" s="1"/>
-      <c r="L162" s="1"/>
-      <c r="M162" s="1"/>
-      <c r="N162" s="1"/>
+      <c r="C162" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="J162" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K162" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="M162" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N162" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="O162" s="1"/>
-      <c r="P162" s="1"/>
-      <c r="Q162" s="1"/>
-      <c r="R162" s="1"/>
-      <c r="S162" s="1"/>
-      <c r="T162" s="1"/>
-      <c r="U162" s="1"/>
+      <c r="P162" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q162" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="R162" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="S162" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="T162" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="U162" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="V162" s="1"/>
       <c r="W162" s="1"/>
       <c r="X162" s="1"/>
@@ -19416,7 +19434,9 @@
       <c r="AD162" s="1"/>
       <c r="AE162" s="1"/>
       <c r="AF162" s="1"/>
-      <c r="AG162" s="1"/>
+      <c r="AG162" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="AH162" s="1"/>
       <c r="AI162" s="1"/>
       <c r="AJ162" s="1"/>
@@ -19436,12 +19456,21 @@
       <c r="AX162" s="1"/>
       <c r="AY162" s="1"/>
       <c r="AZ162" s="1"/>
-      <c r="BA162" s="1"/>
-      <c r="BB162" s="1"/>
-      <c r="BC162" s="1"/>
-      <c r="BD162" s="1"/>
-      <c r="BE162" s="1"/>
-      <c r="BF162" s="1"/>
+      <c r="BA162" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB162" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD162" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE162" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF162" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="BG162" s="1"/>
       <c r="BH162" s="1"/>
       <c r="BI162" s="11"/>
@@ -19467,12 +19496,14 @@
       <c r="CC162" s="1"/>
       <c r="CD162" s="1"/>
       <c r="CE162" s="1"/>
-      <c r="CF162" s="1"/>
-      <c r="CG162" s="1"/>
+      <c r="CF162" s="18"/>
+      <c r="CG162" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row customFormat="1" r="163" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>365</v>
@@ -19485,12 +19516,8 @@
       </c>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
-      <c r="G163" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>242</v>
-      </c>
+      <c r="G163" s="3"/>
+      <c r="H163" s="1"/>
       <c r="I163" s="1" t="s">
         <v>431</v>
       </c>
@@ -19501,7 +19528,7 @@
         <v>349</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="M163" s="2" t="s">
         <v>28</v>
@@ -19561,21 +19588,12 @@
       <c r="AX163" s="1"/>
       <c r="AY163" s="1"/>
       <c r="AZ163" s="1"/>
-      <c r="BA163" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BB163" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD163" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE163" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF163" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="BA163" s="1"/>
+      <c r="BB163" s="1"/>
+      <c r="BC163" s="12"/>
+      <c r="BD163" s="1"/>
+      <c r="BE163" s="1"/>
+      <c r="BF163" s="1"/>
       <c r="BG163" s="1"/>
       <c r="BH163" s="1"/>
       <c r="BI163" s="11"/>
@@ -19608,42 +19626,44 @@
     </row>
     <row customFormat="1" r="164" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C164" s="28" t="s">
-        <v>385</v>
+        <v>462</v>
       </c>
       <c r="D164" s="11" t="s">
         <v>362</v>
       </c>
       <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
+      <c r="F164" s="3" t="s">
+        <v>362</v>
+      </c>
       <c r="G164" s="3" t="s">
-        <v>6</v>
+        <v>241</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>6</v>
+        <v>242</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>431</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="M164" s="2" t="s">
-        <v>28</v>
+        <v>370</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>235</v>
+        <v>371</v>
       </c>
       <c r="O164" s="1"/>
       <c r="P164" s="1" t="s">
@@ -19676,7 +19696,7 @@
       <c r="AE164" s="1"/>
       <c r="AF164" s="1"/>
       <c r="AG164" s="1" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="AH164" s="1"/>
       <c r="AI164" s="1"/>
@@ -19697,21 +19717,12 @@
       <c r="AX164" s="1"/>
       <c r="AY164" s="1"/>
       <c r="AZ164" s="1"/>
-      <c r="BA164" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BB164" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD164" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE164" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF164" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="BA164" s="1"/>
+      <c r="BB164" s="1"/>
+      <c r="BC164" s="12"/>
+      <c r="BD164" s="1"/>
+      <c r="BE164" s="1"/>
+      <c r="BF164" s="1"/>
       <c r="BG164" s="1"/>
       <c r="BH164" s="1"/>
       <c r="BI164" s="11"/>
@@ -19743,8 +19754,8 @@
       </c>
     </row>
     <row customFormat="1" r="165" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
-        <v>250</v>
+      <c r="A165" s="7" t="s">
+        <v>252</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>365</v>
@@ -19757,8 +19768,12 @@
       </c>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
-      <c r="G165" s="3"/>
-      <c r="H165" s="1"/>
+      <c r="G165" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="I165" s="1" t="s">
         <v>431</v>
       </c>
@@ -19829,12 +19844,21 @@
       <c r="AX165" s="1"/>
       <c r="AY165" s="1"/>
       <c r="AZ165" s="1"/>
-      <c r="BA165" s="1"/>
-      <c r="BB165" s="1"/>
-      <c r="BC165" s="12"/>
-      <c r="BD165" s="1"/>
-      <c r="BE165" s="1"/>
-      <c r="BF165" s="1"/>
+      <c r="BA165" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB165" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD165" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE165" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF165" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="BG165" s="1"/>
       <c r="BH165" s="1"/>
       <c r="BI165" s="11"/>
@@ -19866,45 +19890,39 @@
       </c>
     </row>
     <row customFormat="1" r="166" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>251</v>
+      <c r="A166" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C166" s="28" t="s">
-        <v>437</v>
+        <v>385</v>
       </c>
       <c r="D166" s="11" t="s">
         <v>362</v>
       </c>
       <c r="E166" s="3"/>
-      <c r="F166" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="G166" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H166" s="1" t="s">
-        <v>242</v>
-      </c>
+      <c r="F166" s="3"/>
+      <c r="G166" s="3"/>
+      <c r="H166" s="1"/>
       <c r="I166" s="1" t="s">
         <v>431</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>374</v>
+        <v>315</v>
       </c>
       <c r="K166" s="2" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="L166" s="1" t="s">
-        <v>373</v>
+        <v>316</v>
       </c>
       <c r="M166" s="2" t="s">
-        <v>370</v>
+        <v>28</v>
       </c>
       <c r="N166" s="1" t="s">
-        <v>371</v>
+        <v>235</v>
       </c>
       <c r="O166" s="1"/>
       <c r="P166" s="1" t="s">
@@ -19937,7 +19955,7 @@
       <c r="AE166" s="1"/>
       <c r="AF166" s="1"/>
       <c r="AG166" s="1" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="AH166" s="1"/>
       <c r="AI166" s="1"/>
@@ -19958,12 +19976,21 @@
       <c r="AX166" s="1"/>
       <c r="AY166" s="1"/>
       <c r="AZ166" s="1"/>
-      <c r="BA166" s="1"/>
-      <c r="BB166" s="1"/>
-      <c r="BC166" s="12"/>
-      <c r="BD166" s="1"/>
-      <c r="BE166" s="1"/>
-      <c r="BF166" s="1"/>
+      <c r="BA166" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB166" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD166" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE166" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BF166" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="BG166" s="1"/>
       <c r="BH166" s="1"/>
       <c r="BI166" s="11"/>
@@ -19996,7 +20023,7 @@
     </row>
     <row customFormat="1" r="167" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>365</v>
@@ -20009,12 +20036,8 @@
       </c>
       <c r="E167" s="3"/>
       <c r="F167" s="3"/>
-      <c r="G167" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H167" s="1" t="s">
-        <v>242</v>
-      </c>
+      <c r="G167" s="3"/>
+      <c r="H167" s="1"/>
       <c r="I167" s="1" t="s">
         <v>431</v>
       </c>
@@ -20132,32 +20155,38 @@
     </row>
     <row customFormat="1" r="168" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C168" s="28" t="s">
-        <v>385</v>
+        <v>463</v>
       </c>
       <c r="D168" s="11" t="s">
         <v>362</v>
       </c>
       <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
-      <c r="H168" s="1"/>
+      <c r="F168" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="I168" s="1" t="s">
         <v>431</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>315</v>
+        <v>386</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>349</v>
+        <v>387</v>
       </c>
       <c r="L168" s="1" t="s">
-        <v>316</v>
+        <v>244</v>
       </c>
       <c r="M168" s="2" t="s">
         <v>28</v>
@@ -20196,7 +20225,7 @@
       <c r="AE168" s="1"/>
       <c r="AF168" s="1"/>
       <c r="AG168" s="1" t="s">
-        <v>351</v>
+        <v>388</v>
       </c>
       <c r="AH168" s="1"/>
       <c r="AI168" s="1"/>
@@ -20248,14 +20277,14 @@
       <c r="BT168" s="1"/>
       <c r="BU168" s="1"/>
       <c r="BV168" s="1"/>
-      <c r="BW168" s="1"/>
-      <c r="BX168" s="1"/>
-      <c r="BY168" s="1"/>
-      <c r="BZ168" s="1"/>
-      <c r="CA168" s="1"/>
-      <c r="CB168" s="1"/>
-      <c r="CC168" s="1"/>
-      <c r="CD168" s="1"/>
+      <c r="BW168" s="12"/>
+      <c r="BX168" s="12"/>
+      <c r="BY168" s="12"/>
+      <c r="BZ168" s="12"/>
+      <c r="CA168" s="12"/>
+      <c r="CB168" s="12"/>
+      <c r="CC168" s="12"/>
+      <c r="CD168" s="12"/>
       <c r="CE168" s="1"/>
       <c r="CF168" s="18"/>
       <c r="CG168" t="s">
@@ -20264,58 +20293,40 @@
     </row>
     <row customFormat="1" r="169" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C169" s="28" t="s">
-        <v>385</v>
+      <c r="C169" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="D169" s="11" t="s">
-        <v>362</v>
+        <v>3</v>
       </c>
       <c r="E169" s="3"/>
       <c r="F169" s="3"/>
-      <c r="G169" s="3"/>
-      <c r="H169" s="1"/>
+      <c r="G169" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="I169" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="J169" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="K169" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="L169" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="M169" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N169" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="J169" s="1"/>
+      <c r="K169" s="2"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="1"/>
       <c r="O169" s="1"/>
-      <c r="P169" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q169" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="R169" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="S169" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="T169" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="U169" s="1" t="s">
-        <v>246</v>
-      </c>
+      <c r="P169" s="1"/>
+      <c r="Q169" s="11"/>
+      <c r="R169" s="10"/>
+      <c r="S169" s="10"/>
+      <c r="T169" s="1"/>
+      <c r="U169" s="1"/>
       <c r="V169" s="1"/>
       <c r="W169" s="1"/>
       <c r="X169" s="1"/>
@@ -20327,9 +20338,7 @@
       <c r="AD169" s="1"/>
       <c r="AE169" s="1"/>
       <c r="AF169" s="1"/>
-      <c r="AG169" s="1" t="s">
-        <v>351</v>
-      </c>
+      <c r="AG169" s="1"/>
       <c r="AH169" s="1"/>
       <c r="AI169" s="1"/>
       <c r="AJ169" s="1"/>
@@ -20349,24 +20358,18 @@
       <c r="AX169" s="1"/>
       <c r="AY169" s="1"/>
       <c r="AZ169" s="1"/>
-      <c r="BA169" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BB169" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD169" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE169" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF169" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="BA169" s="1"/>
+      <c r="BB169" s="4"/>
+      <c r="BD169" s="2"/>
+      <c r="BE169" s="3"/>
+      <c r="BF169" s="2"/>
       <c r="BG169" s="1"/>
-      <c r="BH169" s="1"/>
-      <c r="BI169" s="11"/>
+      <c r="BH169" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="BI169" s="11" t="s">
+        <v>352</v>
+      </c>
       <c r="BJ169" s="1"/>
       <c r="BK169" s="1"/>
       <c r="BL169" s="1"/>
@@ -20380,54 +20383,52 @@
       <c r="BT169" s="1"/>
       <c r="BU169" s="1"/>
       <c r="BV169" s="1"/>
-      <c r="BW169" s="1"/>
-      <c r="BX169" s="1"/>
-      <c r="BY169" s="1"/>
-      <c r="BZ169" s="1"/>
-      <c r="CA169" s="1"/>
-      <c r="CB169" s="1"/>
-      <c r="CC169" s="1"/>
-      <c r="CD169" s="1"/>
+      <c r="BW169" s="12"/>
+      <c r="BX169" s="12"/>
+      <c r="BY169" s="12"/>
+      <c r="BZ169" s="12"/>
+      <c r="CA169" s="12"/>
+      <c r="CB169" s="12"/>
+      <c r="CC169" s="12"/>
+      <c r="CD169" s="12"/>
       <c r="CE169" s="1"/>
       <c r="CF169" s="18"/>
       <c r="CG169" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row customFormat="1" r="170" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C170" s="28" t="s">
-        <v>436</v>
-      </c>
-      <c r="D170" s="11" t="s">
-        <v>362</v>
+        <v>285</v>
+      </c>
+      <c r="D170" s="28" t="s">
+        <v>389</v>
       </c>
       <c r="E170" s="3"/>
-      <c r="F170" s="11" t="s">
-        <v>362</v>
-      </c>
+      <c r="F170" s="3"/>
       <c r="G170" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H170" s="1" t="s">
-        <v>242</v>
+        <v>53</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="I170" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="J170" s="1" t="s">
-        <v>386</v>
+      <c r="J170" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>387</v>
+        <v>1</v>
       </c>
       <c r="L170" s="1" t="s">
-        <v>244</v>
+        <v>5</v>
       </c>
       <c r="M170" s="2" t="s">
         <v>28</v>
@@ -20439,21 +20440,11 @@
       <c r="P170" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q170" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="R170" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="S170" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="T170" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="U170" s="1" t="s">
-        <v>246</v>
-      </c>
+      <c r="Q170" s="11"/>
+      <c r="R170" s="1"/>
+      <c r="S170" s="1"/>
+      <c r="T170" s="1"/>
+      <c r="U170" s="1"/>
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
@@ -20465,9 +20456,7 @@
       <c r="AD170" s="1"/>
       <c r="AE170" s="1"/>
       <c r="AF170" s="1"/>
-      <c r="AG170" s="1" t="s">
-        <v>388</v>
-      </c>
+      <c r="AG170" s="1"/>
       <c r="AH170" s="1"/>
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
@@ -20488,25 +20477,25 @@
       <c r="AY170" s="1"/>
       <c r="AZ170" s="1"/>
       <c r="BA170" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BB170" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BD170" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE170" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF170" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="BB170" s="4"/>
+      <c r="BD170" s="2"/>
+      <c r="BE170" s="3"/>
+      <c r="BF170" s="2"/>
       <c r="BG170" s="1"/>
-      <c r="BH170" s="1"/>
-      <c r="BI170" s="11"/>
-      <c r="BJ170" s="1"/>
-      <c r="BK170" s="1"/>
+      <c r="BH170" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="BI170" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ170" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK170" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="BL170" s="1"/>
       <c r="BM170" s="1"/>
       <c r="BN170" s="1"/>
@@ -20529,45 +20518,57 @@
       <c r="CE170" s="1"/>
       <c r="CF170" s="18"/>
       <c r="CG170" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row customFormat="1" r="171" spans="1:85" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="30" r="171" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C171" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D171" s="11" t="s">
-        <v>3</v>
+      <c r="C171" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="D171" s="28" t="s">
+        <v>389</v>
       </c>
       <c r="E171" s="3"/>
       <c r="F171" s="3"/>
-      <c r="G171" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H171" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
       <c r="I171" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="J171" s="1"/>
-      <c r="K171" s="2"/>
-      <c r="L171" s="1"/>
+      <c r="J171" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="M171" s="2"/>
       <c r="N171" s="1"/>
       <c r="O171" s="1"/>
       <c r="P171" s="1"/>
-      <c r="Q171" s="11"/>
-      <c r="R171" s="10"/>
-      <c r="S171" s="10"/>
-      <c r="T171" s="1"/>
-      <c r="U171" s="1"/>
+      <c r="Q171" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="R171" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="S171" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="T171" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="U171" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
@@ -20579,7 +20580,9 @@
       <c r="AD171" s="1"/>
       <c r="AE171" s="1"/>
       <c r="AF171" s="1"/>
-      <c r="AG171" s="1"/>
+      <c r="AG171" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="AH171" s="1"/>
       <c r="AI171" s="1"/>
       <c r="AJ171" s="1"/>
@@ -20605,16 +20608,14 @@
       <c r="BE171" s="3"/>
       <c r="BF171" s="2"/>
       <c r="BG171" s="1"/>
-      <c r="BH171" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="BI171" s="11" t="s">
-        <v>352</v>
-      </c>
+      <c r="BH171" s="1"/>
+      <c r="BI171" s="11"/>
       <c r="BJ171" s="1"/>
       <c r="BK171" s="1"/>
       <c r="BL171" s="1"/>
-      <c r="BM171" s="1"/>
+      <c r="BM171" s="1" t="s">
+        <v>294</v>
+      </c>
       <c r="BN171" s="1"/>
       <c r="BO171" s="1"/>
       <c r="BP171" s="1"/>
@@ -20638,34 +20639,32 @@
         <v>364</v>
       </c>
     </row>
-    <row customFormat="1" r="172" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A172" s="7" t="s">
-        <v>283</v>
+    <row customFormat="1" ht="30" r="172" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>437</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C172" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="D172" s="28" t="s">
-        <v>389</v>
-      </c>
-      <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
-      <c r="G172" s="3" t="s">
+      <c r="C172" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="2" t="s">
         <v>53</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I172" s="1" t="s">
-        <v>431</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="I172" s="1"/>
       <c r="J172" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K172" s="2" t="s">
+      <c r="K172" t="s">
         <v>1</v>
       </c>
       <c r="L172" s="1" t="s">
@@ -20681,7 +20680,7 @@
       <c r="P172" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q172" s="11"/>
+      <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
       <c r="S172" s="1"/>
       <c r="T172" s="1"/>
@@ -20718,25 +20717,22 @@
       <c r="AY172" s="1"/>
       <c r="AZ172" s="1"/>
       <c r="BA172" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB172" s="4"/>
-      <c r="BD172" s="2"/>
-      <c r="BE172" s="3"/>
-      <c r="BF172" s="2"/>
-      <c r="BG172" s="1"/>
-      <c r="BH172" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="BI172" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="BJ172" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="BK172" s="1" t="s">
-        <v>353</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="BB172" s="1"/>
+      <c r="BC172" s="1"/>
+      <c r="BD172" s="1"/>
+      <c r="BE172" s="1"/>
+      <c r="BF172" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="BG172" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="BH172" s="1"/>
+      <c r="BI172" s="1"/>
+      <c r="BJ172" s="1"/>
+      <c r="BK172" s="1"/>
       <c r="BL172" s="1"/>
       <c r="BM172" s="1"/>
       <c r="BN172" s="1"/>
@@ -20748,68 +20744,66 @@
       <c r="BT172" s="1"/>
       <c r="BU172" s="1"/>
       <c r="BV172" s="1"/>
-      <c r="BW172" s="12"/>
-      <c r="BX172" s="12"/>
-      <c r="BY172" s="12"/>
-      <c r="BZ172" s="12"/>
-      <c r="CA172" s="12"/>
-      <c r="CB172" s="12"/>
-      <c r="CC172" s="12"/>
-      <c r="CD172" s="12"/>
+      <c r="BW172" s="1"/>
+      <c r="BX172" s="1"/>
+      <c r="BY172" s="1"/>
+      <c r="BZ172" s="1"/>
+      <c r="CA172" s="1"/>
+      <c r="CB172" s="1"/>
+      <c r="CC172" s="1"/>
+      <c r="CD172" s="1"/>
       <c r="CE172" s="1"/>
-      <c r="CF172" s="18"/>
+      <c r="CF172" s="1"/>
       <c r="CG172" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row customFormat="1" ht="30" r="173" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A173" s="7" t="s">
-        <v>288</v>
+      <c r="A173" s="2" t="s">
+        <v>441</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C173" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="D173" s="28" t="s">
-        <v>389</v>
-      </c>
-      <c r="E173" s="3"/>
-      <c r="F173" s="3"/>
-      <c r="G173" s="3"/>
-      <c r="H173" s="3"/>
-      <c r="I173" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="C173" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H173" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I173" s="1"/>
       <c r="J173" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="K173" s="2" t="s">
-        <v>293</v>
+        <v>0</v>
+      </c>
+      <c r="K173" t="s">
+        <v>1</v>
       </c>
       <c r="L173" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="M173" s="2"/>
-      <c r="N173" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="M173" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N173" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="O173" s="1"/>
-      <c r="P173" s="1"/>
-      <c r="Q173" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="R173" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="S173" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="T173" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="U173" s="1" t="s">
-        <v>296</v>
-      </c>
+      <c r="P173" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q173" s="1"/>
+      <c r="R173" s="1"/>
+      <c r="S173" s="1"/>
+      <c r="T173" s="1"/>
+      <c r="U173" s="1"/>
       <c r="V173" s="1"/>
       <c r="W173" s="1"/>
       <c r="X173" s="1"/>
@@ -20821,9 +20815,7 @@
       <c r="AD173" s="1"/>
       <c r="AE173" s="1"/>
       <c r="AF173" s="1"/>
-      <c r="AG173" s="1" t="s">
-        <v>289</v>
-      </c>
+      <c r="AG173" s="1"/>
       <c r="AH173" s="1"/>
       <c r="AI173" s="1"/>
       <c r="AJ173" s="1"/>
@@ -20843,20 +20835,25 @@
       <c r="AX173" s="1"/>
       <c r="AY173" s="1"/>
       <c r="AZ173" s="1"/>
-      <c r="BA173" s="1"/>
-      <c r="BB173" s="4"/>
-      <c r="BD173" s="2"/>
-      <c r="BE173" s="3"/>
-      <c r="BF173" s="2"/>
-      <c r="BG173" s="1"/>
+      <c r="BA173" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="BB173" s="1"/>
+      <c r="BC173" s="1"/>
+      <c r="BD173" s="1"/>
+      <c r="BE173" s="1"/>
+      <c r="BF173" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="BG173" s="4" t="s">
+        <v>440</v>
+      </c>
       <c r="BH173" s="1"/>
-      <c r="BI173" s="11"/>
+      <c r="BI173" s="1"/>
       <c r="BJ173" s="1"/>
       <c r="BK173" s="1"/>
       <c r="BL173" s="1"/>
-      <c r="BM173" s="1" t="s">
-        <v>294</v>
-      </c>
+      <c r="BM173" s="1"/>
       <c r="BN173" s="1"/>
       <c r="BO173" s="1"/>
       <c r="BP173" s="1"/>
@@ -20866,23 +20863,23 @@
       <c r="BT173" s="1"/>
       <c r="BU173" s="1"/>
       <c r="BV173" s="1"/>
-      <c r="BW173" s="12"/>
-      <c r="BX173" s="12"/>
-      <c r="BY173" s="12"/>
-      <c r="BZ173" s="12"/>
-      <c r="CA173" s="12"/>
-      <c r="CB173" s="12"/>
-      <c r="CC173" s="12"/>
-      <c r="CD173" s="12"/>
+      <c r="BW173" s="1"/>
+      <c r="BX173" s="1"/>
+      <c r="BY173" s="1"/>
+      <c r="BZ173" s="1"/>
+      <c r="CA173" s="1"/>
+      <c r="CB173" s="1"/>
+      <c r="CC173" s="1"/>
+      <c r="CD173" s="1"/>
       <c r="CE173" s="1"/>
-      <c r="CF173" s="18"/>
+      <c r="CF173" s="1"/>
       <c r="CG173" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row customFormat="1" ht="30" r="174" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>365</v>
@@ -20958,17 +20955,17 @@
       <c r="AY174" s="1"/>
       <c r="AZ174" s="1"/>
       <c r="BA174" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB174" s="1"/>
       <c r="BC174" s="1"/>
       <c r="BD174" s="1"/>
       <c r="BE174" s="1"/>
       <c r="BF174" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="BG174" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH174" s="1"/>
       <c r="BI174" s="1"/>
@@ -20999,9 +20996,9 @@
         <v>366</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="175" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="175" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>365</v>
@@ -21077,17 +21074,17 @@
       <c r="AY175" s="1"/>
       <c r="AZ175" s="1"/>
       <c r="BA175" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB175" s="1"/>
       <c r="BC175" s="1"/>
       <c r="BD175" s="1"/>
       <c r="BE175" s="1"/>
       <c r="BF175" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="BG175" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH175" s="1"/>
       <c r="BI175" s="1"/>
@@ -21118,9 +21115,9 @@
         <v>366</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="176" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="176" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>365</v>
@@ -21196,17 +21193,17 @@
       <c r="AY176" s="1"/>
       <c r="AZ176" s="1"/>
       <c r="BA176" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB176" s="1"/>
       <c r="BC176" s="1"/>
       <c r="BD176" s="1"/>
       <c r="BE176" s="1"/>
       <c r="BF176" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="BG176" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH176" s="1"/>
       <c r="BI176" s="1"/>
@@ -21239,7 +21236,7 @@
     </row>
     <row customFormat="1" r="177" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>365</v>
@@ -21315,17 +21312,17 @@
       <c r="AY177" s="1"/>
       <c r="AZ177" s="1"/>
       <c r="BA177" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB177" s="1"/>
       <c r="BC177" s="1"/>
       <c r="BD177" s="1"/>
       <c r="BE177" s="1"/>
       <c r="BF177" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="BG177" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH177" s="1"/>
       <c r="BI177" s="1"/>
@@ -21356,19 +21353,17 @@
         <v>366</v>
       </c>
     </row>
-    <row customFormat="1" r="178" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="178" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D178" s="1"/>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
       <c r="G178" s="2" t="s">
@@ -21434,17 +21429,17 @@
       <c r="AY178" s="1"/>
       <c r="AZ178" s="1"/>
       <c r="BA178" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB178" s="1"/>
       <c r="BC178" s="1"/>
       <c r="BD178" s="1"/>
       <c r="BE178" s="1"/>
       <c r="BF178" s="1" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="BG178" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH178" s="1"/>
       <c r="BI178" s="1"/>
@@ -21475,19 +21470,17 @@
         <v>366</v>
       </c>
     </row>
-    <row customFormat="1" r="179" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="179" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D179" s="1"/>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
       <c r="G179" s="2" t="s">
@@ -21553,17 +21546,17 @@
       <c r="AY179" s="1"/>
       <c r="AZ179" s="1"/>
       <c r="BA179" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB179" s="1"/>
       <c r="BC179" s="1"/>
       <c r="BD179" s="1"/>
       <c r="BE179" s="1"/>
       <c r="BF179" s="1" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="BG179" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH179" s="1"/>
       <c r="BI179" s="1"/>
@@ -21596,7 +21589,7 @@
     </row>
     <row customFormat="1" ht="30" r="180" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>365</v>
@@ -21670,17 +21663,17 @@
       <c r="AY180" s="1"/>
       <c r="AZ180" s="1"/>
       <c r="BA180" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB180" s="1"/>
       <c r="BC180" s="1"/>
       <c r="BD180" s="1"/>
       <c r="BE180" s="1"/>
       <c r="BF180" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="BG180" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH180" s="1"/>
       <c r="BI180" s="1"/>
@@ -21711,9 +21704,9 @@
         <v>366</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="181" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="181" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>365</v>
@@ -21787,17 +21780,17 @@
       <c r="AY181" s="1"/>
       <c r="AZ181" s="1"/>
       <c r="BA181" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB181" s="1"/>
       <c r="BC181" s="1"/>
       <c r="BD181" s="1"/>
       <c r="BE181" s="1"/>
       <c r="BF181" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="BG181" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH181" s="1"/>
       <c r="BI181" s="1"/>
@@ -21828,9 +21821,9 @@
         <v>366</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="182" spans="1:85" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="182" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>365</v>
@@ -21904,17 +21897,17 @@
       <c r="AY182" s="1"/>
       <c r="AZ182" s="1"/>
       <c r="BA182" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB182" s="1"/>
       <c r="BC182" s="1"/>
       <c r="BD182" s="1"/>
       <c r="BE182" s="1"/>
       <c r="BF182" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="BG182" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH182" s="1"/>
       <c r="BI182" s="1"/>
@@ -21947,7 +21940,7 @@
     </row>
     <row customFormat="1" r="183" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>365</v>
@@ -22021,17 +22014,17 @@
       <c r="AY183" s="1"/>
       <c r="AZ183" s="1"/>
       <c r="BA183" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB183" s="1"/>
       <c r="BC183" s="1"/>
       <c r="BD183" s="1"/>
       <c r="BE183" s="1"/>
       <c r="BF183" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="BG183" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="BH183" s="1"/>
       <c r="BI183" s="1"/>
@@ -22059,20 +22052,22 @@
       <c r="CE183" s="1"/>
       <c r="CF183" s="1"/>
       <c r="CG183" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row customFormat="1" r="184" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D184" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
       <c r="G184" s="2" t="s">
@@ -22138,18 +22133,14 @@
       <c r="AY184" s="1"/>
       <c r="AZ184" s="1"/>
       <c r="BA184" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB184" s="1"/>
       <c r="BC184" s="1"/>
       <c r="BD184" s="1"/>
       <c r="BE184" s="1"/>
-      <c r="BF184" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="BG184" s="4" t="s">
-        <v>447</v>
-      </c>
+      <c r="BF184" s="1"/>
+      <c r="BG184" s="4"/>
       <c r="BH184" s="1"/>
       <c r="BI184" s="1"/>
       <c r="BJ184" s="1"/>
@@ -22181,7 +22172,7 @@
     </row>
     <row customFormat="1" r="185" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>365</v>
@@ -22255,18 +22246,16 @@
       <c r="AY185" s="1"/>
       <c r="AZ185" s="1"/>
       <c r="BA185" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="BB185" s="1"/>
       <c r="BC185" s="1"/>
       <c r="BD185" s="1"/>
       <c r="BE185" s="1"/>
       <c r="BF185" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="BG185" s="4" t="s">
-        <v>447</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="BG185" s="4"/>
       <c r="BH185" s="1"/>
       <c r="BI185" s="1"/>
       <c r="BJ185" s="1"/>
@@ -22293,50 +22282,26 @@
       <c r="CE185" s="1"/>
       <c r="CF185" s="1"/>
       <c r="CG185" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row customFormat="1" r="186" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A186" s="7"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
-      <c r="G186" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H186" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="G186" s="1"/>
+      <c r="H186" s="1"/>
       <c r="I186" s="1"/>
-      <c r="J186" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K186" t="s">
-        <v>1</v>
-      </c>
-      <c r="L186" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M186" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N186" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+      <c r="L186" s="1"/>
+      <c r="M186" s="1"/>
+      <c r="N186" s="1"/>
       <c r="O186" s="1"/>
-      <c r="P186" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="P186" s="1"/>
       <c r="Q186" s="1"/>
       <c r="R186" s="1"/>
       <c r="S186" s="1"/>
@@ -22373,17 +22338,15 @@
       <c r="AX186" s="1"/>
       <c r="AY186" s="1"/>
       <c r="AZ186" s="1"/>
-      <c r="BA186" s="1" t="s">
-        <v>445</v>
-      </c>
+      <c r="BA186" s="1"/>
       <c r="BB186" s="1"/>
       <c r="BC186" s="1"/>
       <c r="BD186" s="1"/>
       <c r="BE186" s="1"/>
       <c r="BF186" s="1"/>
-      <c r="BG186" s="4"/>
+      <c r="BG186" s="1"/>
       <c r="BH186" s="1"/>
-      <c r="BI186" s="1"/>
+      <c r="BI186" s="11"/>
       <c r="BJ186" s="1"/>
       <c r="BK186" s="1"/>
       <c r="BL186" s="1"/>
@@ -22407,49 +22370,25 @@
       <c r="CD186" s="1"/>
       <c r="CE186" s="1"/>
       <c r="CF186" s="1"/>
-      <c r="CG186" t="s">
-        <v>366</v>
-      </c>
+      <c r="CG186" s="1"/>
     </row>
     <row customFormat="1" r="187" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>329</v>
-      </c>
+      <c r="A187" s="7"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
-      <c r="G187" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H187" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
       <c r="I187" s="1"/>
-      <c r="J187" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K187" t="s">
-        <v>1</v>
-      </c>
-      <c r="L187" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M187" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N187" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1"/>
       <c r="O187" s="1"/>
-      <c r="P187" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="P187" s="1"/>
       <c r="Q187" s="1"/>
       <c r="R187" s="1"/>
       <c r="S187" s="1"/>
@@ -22486,19 +22425,15 @@
       <c r="AX187" s="1"/>
       <c r="AY187" s="1"/>
       <c r="AZ187" s="1"/>
-      <c r="BA187" s="1" t="s">
-        <v>445</v>
-      </c>
+      <c r="BA187" s="1"/>
       <c r="BB187" s="1"/>
       <c r="BC187" s="1"/>
       <c r="BD187" s="1"/>
       <c r="BE187" s="1"/>
-      <c r="BF187" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BG187" s="4"/>
+      <c r="BF187" s="1"/>
+      <c r="BG187" s="1"/>
       <c r="BH187" s="1"/>
-      <c r="BI187" s="1"/>
+      <c r="BI187" s="11"/>
       <c r="BJ187" s="1"/>
       <c r="BK187" s="1"/>
       <c r="BL187" s="1"/>
@@ -22522,9 +22457,7 @@
       <c r="CD187" s="1"/>
       <c r="CE187" s="1"/>
       <c r="CF187" s="1"/>
-      <c r="CG187" t="s">
-        <v>366</v>
-      </c>
+      <c r="CG187" s="1"/>
     </row>
     <row customFormat="1" r="188" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
@@ -22616,7 +22549,7 @@
     <row customFormat="1" r="189" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A189" s="7"/>
       <c r="B189" s="1"/>
-      <c r="C189" s="1"/>
+      <c r="C189" s="11"/>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
@@ -22703,7 +22636,7 @@
     <row customFormat="1" r="190" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A190" s="7"/>
       <c r="B190" s="1"/>
-      <c r="C190" s="1"/>
+      <c r="C190" s="11"/>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
@@ -24441,178 +24374,178 @@
       <c r="CG209" s="1"/>
     </row>
     <row customFormat="1" r="210" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A210" s="7"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="11"/>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
-      <c r="G210" s="1"/>
-      <c r="H210" s="1"/>
-      <c r="I210" s="1"/>
-      <c r="J210" s="1"/>
-      <c r="K210" s="1"/>
-      <c r="L210" s="1"/>
-      <c r="M210" s="1"/>
-      <c r="N210" s="1"/>
-      <c r="O210" s="1"/>
-      <c r="P210" s="1"/>
-      <c r="Q210" s="1"/>
-      <c r="R210" s="1"/>
-      <c r="S210" s="1"/>
-      <c r="T210" s="1"/>
-      <c r="U210" s="1"/>
-      <c r="V210" s="1"/>
-      <c r="W210" s="1"/>
-      <c r="X210" s="1"/>
-      <c r="Y210" s="1"/>
-      <c r="Z210" s="1"/>
-      <c r="AA210" s="1"/>
-      <c r="AB210" s="1"/>
-      <c r="AC210" s="1"/>
-      <c r="AD210" s="1"/>
-      <c r="AE210" s="1"/>
-      <c r="AF210" s="1"/>
-      <c r="AG210" s="1"/>
-      <c r="AH210" s="1"/>
-      <c r="AI210" s="1"/>
-      <c r="AJ210" s="1"/>
-      <c r="AK210" s="1"/>
-      <c r="AL210" s="1"/>
-      <c r="AM210" s="1"/>
-      <c r="AN210" s="1"/>
-      <c r="AO210" s="1"/>
-      <c r="AP210" s="1"/>
-      <c r="AQ210" s="1"/>
-      <c r="AR210" s="1"/>
-      <c r="AS210" s="1"/>
-      <c r="AT210" s="1"/>
-      <c r="AU210" s="1"/>
-      <c r="AV210" s="1"/>
-      <c r="AW210" s="1"/>
-      <c r="AX210" s="1"/>
-      <c r="AY210" s="1"/>
-      <c r="AZ210" s="1"/>
-      <c r="BA210" s="1"/>
-      <c r="BB210" s="1"/>
-      <c r="BC210" s="1"/>
-      <c r="BD210" s="1"/>
-      <c r="BE210" s="1"/>
-      <c r="BF210" s="1"/>
-      <c r="BG210" s="1"/>
-      <c r="BH210" s="1"/>
-      <c r="BI210" s="11"/>
-      <c r="BJ210" s="1"/>
-      <c r="BK210" s="1"/>
-      <c r="BL210" s="1"/>
-      <c r="BM210" s="1"/>
-      <c r="BN210" s="1"/>
-      <c r="BO210" s="1"/>
-      <c r="BP210" s="1"/>
-      <c r="BQ210" s="1"/>
-      <c r="BR210" s="1"/>
-      <c r="BS210" s="1"/>
-      <c r="BT210" s="1"/>
-      <c r="BU210" s="1"/>
-      <c r="BV210" s="1"/>
-      <c r="BW210" s="1"/>
-      <c r="BX210" s="1"/>
-      <c r="BY210" s="1"/>
-      <c r="BZ210" s="1"/>
-      <c r="CA210" s="1"/>
-      <c r="CB210" s="1"/>
-      <c r="CC210" s="1"/>
-      <c r="CD210" s="1"/>
-      <c r="CE210" s="1"/>
-      <c r="CF210" s="1"/>
-      <c r="CG210" s="1"/>
+      <c r="A210" s="8"/>
+      <c r="B210" s="2"/>
+      <c r="C210" s="3"/>
+      <c r="D210" s="2"/>
+      <c r="E210" s="2"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="2"/>
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+      <c r="J210" s="2"/>
+      <c r="K210" s="2"/>
+      <c r="L210" s="2"/>
+      <c r="M210" s="2"/>
+      <c r="N210" s="2"/>
+      <c r="O210" s="2"/>
+      <c r="P210" s="2"/>
+      <c r="Q210" s="2"/>
+      <c r="R210" s="2"/>
+      <c r="S210" s="2"/>
+      <c r="T210" s="2"/>
+      <c r="U210" s="2"/>
+      <c r="V210" s="2"/>
+      <c r="W210" s="2"/>
+      <c r="X210" s="2"/>
+      <c r="Y210" s="2"/>
+      <c r="Z210" s="2"/>
+      <c r="AA210" s="2"/>
+      <c r="AB210" s="2"/>
+      <c r="AC210" s="2"/>
+      <c r="AD210" s="2"/>
+      <c r="AE210" s="2"/>
+      <c r="AF210" s="2"/>
+      <c r="AG210" s="2"/>
+      <c r="AH210" s="2"/>
+      <c r="AI210" s="2"/>
+      <c r="AJ210" s="2"/>
+      <c r="AK210" s="2"/>
+      <c r="AL210" s="2"/>
+      <c r="AM210" s="2"/>
+      <c r="AN210" s="2"/>
+      <c r="AO210" s="2"/>
+      <c r="AP210" s="2"/>
+      <c r="AQ210" s="2"/>
+      <c r="AR210" s="2"/>
+      <c r="AS210" s="2"/>
+      <c r="AT210" s="2"/>
+      <c r="AU210" s="2"/>
+      <c r="AV210" s="2"/>
+      <c r="AW210" s="2"/>
+      <c r="AX210" s="2"/>
+      <c r="AY210" s="2"/>
+      <c r="AZ210" s="2"/>
+      <c r="BA210" s="2"/>
+      <c r="BB210" s="2"/>
+      <c r="BC210" s="2"/>
+      <c r="BD210" s="2"/>
+      <c r="BE210" s="2"/>
+      <c r="BF210" s="2"/>
+      <c r="BG210" s="2"/>
+      <c r="BH210" s="2"/>
+      <c r="BI210" s="3"/>
+      <c r="BJ210" s="2"/>
+      <c r="BK210" s="2"/>
+      <c r="BL210" s="2"/>
+      <c r="BM210" s="2"/>
+      <c r="BN210" s="2"/>
+      <c r="BO210" s="2"/>
+      <c r="BP210" s="2"/>
+      <c r="BQ210" s="2"/>
+      <c r="BR210" s="2"/>
+      <c r="BS210" s="2"/>
+      <c r="BT210" s="2"/>
+      <c r="BU210" s="2"/>
+      <c r="BV210" s="2"/>
+      <c r="BW210" s="2"/>
+      <c r="BX210" s="2"/>
+      <c r="BY210" s="2"/>
+      <c r="BZ210" s="2"/>
+      <c r="CA210" s="2"/>
+      <c r="CB210" s="2"/>
+      <c r="CC210" s="2"/>
+      <c r="CD210" s="2"/>
+      <c r="CE210" s="2"/>
+      <c r="CF210" s="2"/>
+      <c r="CG210" s="2"/>
     </row>
     <row customFormat="1" r="211" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A211" s="7"/>
-      <c r="B211" s="1"/>
-      <c r="C211" s="11"/>
-      <c r="D211" s="1"/>
-      <c r="E211" s="1"/>
-      <c r="F211" s="1"/>
-      <c r="G211" s="1"/>
-      <c r="H211" s="1"/>
-      <c r="I211" s="1"/>
-      <c r="J211" s="1"/>
-      <c r="K211" s="1"/>
-      <c r="L211" s="1"/>
-      <c r="M211" s="1"/>
-      <c r="N211" s="1"/>
-      <c r="O211" s="1"/>
-      <c r="P211" s="1"/>
-      <c r="Q211" s="1"/>
-      <c r="R211" s="1"/>
-      <c r="S211" s="1"/>
-      <c r="T211" s="1"/>
-      <c r="U211" s="1"/>
-      <c r="V211" s="1"/>
-      <c r="W211" s="1"/>
-      <c r="X211" s="1"/>
-      <c r="Y211" s="1"/>
-      <c r="Z211" s="1"/>
-      <c r="AA211" s="1"/>
-      <c r="AB211" s="1"/>
-      <c r="AC211" s="1"/>
-      <c r="AD211" s="1"/>
-      <c r="AE211" s="1"/>
-      <c r="AF211" s="1"/>
-      <c r="AG211" s="1"/>
-      <c r="AH211" s="1"/>
-      <c r="AI211" s="1"/>
-      <c r="AJ211" s="1"/>
-      <c r="AK211" s="1"/>
-      <c r="AL211" s="1"/>
-      <c r="AM211" s="1"/>
-      <c r="AN211" s="1"/>
-      <c r="AO211" s="1"/>
-      <c r="AP211" s="1"/>
-      <c r="AQ211" s="1"/>
-      <c r="AR211" s="1"/>
-      <c r="AS211" s="1"/>
-      <c r="AT211" s="1"/>
-      <c r="AU211" s="1"/>
-      <c r="AV211" s="1"/>
-      <c r="AW211" s="1"/>
-      <c r="AX211" s="1"/>
-      <c r="AY211" s="1"/>
-      <c r="AZ211" s="1"/>
-      <c r="BA211" s="1"/>
-      <c r="BB211" s="1"/>
-      <c r="BC211" s="1"/>
-      <c r="BD211" s="1"/>
-      <c r="BE211" s="1"/>
-      <c r="BF211" s="1"/>
-      <c r="BG211" s="1"/>
-      <c r="BH211" s="1"/>
-      <c r="BI211" s="11"/>
-      <c r="BJ211" s="1"/>
-      <c r="BK211" s="1"/>
-      <c r="BL211" s="1"/>
-      <c r="BM211" s="1"/>
-      <c r="BN211" s="1"/>
-      <c r="BO211" s="1"/>
-      <c r="BP211" s="1"/>
-      <c r="BQ211" s="1"/>
-      <c r="BR211" s="1"/>
-      <c r="BS211" s="1"/>
-      <c r="BT211" s="1"/>
-      <c r="BU211" s="1"/>
-      <c r="BV211" s="1"/>
-      <c r="BW211" s="1"/>
-      <c r="BX211" s="1"/>
-      <c r="BY211" s="1"/>
-      <c r="BZ211" s="1"/>
-      <c r="CA211" s="1"/>
-      <c r="CB211" s="1"/>
-      <c r="CC211" s="1"/>
-      <c r="CD211" s="1"/>
-      <c r="CE211" s="1"/>
-      <c r="CF211" s="1"/>
-      <c r="CG211" s="1"/>
+      <c r="A211" s="8"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="3"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="2"/>
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+      <c r="J211" s="2"/>
+      <c r="K211" s="2"/>
+      <c r="L211" s="2"/>
+      <c r="M211" s="2"/>
+      <c r="N211" s="2"/>
+      <c r="O211" s="2"/>
+      <c r="P211" s="2"/>
+      <c r="Q211" s="2"/>
+      <c r="R211" s="2"/>
+      <c r="S211" s="2"/>
+      <c r="T211" s="2"/>
+      <c r="U211" s="2"/>
+      <c r="V211" s="2"/>
+      <c r="W211" s="2"/>
+      <c r="X211" s="2"/>
+      <c r="Y211" s="2"/>
+      <c r="Z211" s="2"/>
+      <c r="AA211" s="2"/>
+      <c r="AB211" s="2"/>
+      <c r="AC211" s="2"/>
+      <c r="AD211" s="2"/>
+      <c r="AE211" s="2"/>
+      <c r="AF211" s="2"/>
+      <c r="AG211" s="2"/>
+      <c r="AH211" s="2"/>
+      <c r="AI211" s="2"/>
+      <c r="AJ211" s="2"/>
+      <c r="AK211" s="2"/>
+      <c r="AL211" s="2"/>
+      <c r="AM211" s="2"/>
+      <c r="AN211" s="2"/>
+      <c r="AO211" s="2"/>
+      <c r="AP211" s="2"/>
+      <c r="AQ211" s="2"/>
+      <c r="AR211" s="2"/>
+      <c r="AS211" s="2"/>
+      <c r="AT211" s="2"/>
+      <c r="AU211" s="2"/>
+      <c r="AV211" s="2"/>
+      <c r="AW211" s="2"/>
+      <c r="AX211" s="2"/>
+      <c r="AY211" s="2"/>
+      <c r="AZ211" s="2"/>
+      <c r="BA211" s="2"/>
+      <c r="BB211" s="2"/>
+      <c r="BC211" s="2"/>
+      <c r="BD211" s="2"/>
+      <c r="BE211" s="2"/>
+      <c r="BF211" s="2"/>
+      <c r="BG211" s="2"/>
+      <c r="BH211" s="2"/>
+      <c r="BI211" s="3"/>
+      <c r="BJ211" s="2"/>
+      <c r="BK211" s="2"/>
+      <c r="BL211" s="2"/>
+      <c r="BM211" s="2"/>
+      <c r="BN211" s="2"/>
+      <c r="BO211" s="2"/>
+      <c r="BP211" s="2"/>
+      <c r="BQ211" s="2"/>
+      <c r="BR211" s="2"/>
+      <c r="BS211" s="2"/>
+      <c r="BT211" s="2"/>
+      <c r="BU211" s="2"/>
+      <c r="BV211" s="2"/>
+      <c r="BW211" s="2"/>
+      <c r="BX211" s="2"/>
+      <c r="BY211" s="2"/>
+      <c r="BZ211" s="2"/>
+      <c r="CA211" s="2"/>
+      <c r="CB211" s="2"/>
+      <c r="CC211" s="2"/>
+      <c r="CD211" s="2"/>
+      <c r="CE211" s="2"/>
+      <c r="CF211" s="2"/>
+      <c r="CG211" s="2"/>
     </row>
     <row customFormat="1" r="212" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A212" s="8"/>
@@ -29922,7 +29855,7 @@
       <c r="CG272" s="2"/>
     </row>
     <row customFormat="1" r="273" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A273" s="8"/>
+      <c r="A273" s="2"/>
       <c r="B273" s="2"/>
       <c r="C273" s="3"/>
       <c r="D273" s="2"/>
@@ -30009,7 +29942,7 @@
       <c r="CG273" s="2"/>
     </row>
     <row customFormat="1" r="274" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A274" s="8"/>
+      <c r="A274" s="2"/>
       <c r="B274" s="2"/>
       <c r="C274" s="3"/>
       <c r="D274" s="2"/>
@@ -30792,178 +30725,8 @@
       <c r="CG282" s="2"/>
     </row>
     <row customFormat="1" r="283" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A283" s="2"/>
-      <c r="B283" s="2"/>
-      <c r="C283" s="3"/>
-      <c r="D283" s="2"/>
-      <c r="E283" s="2"/>
-      <c r="F283" s="2"/>
-      <c r="G283" s="2"/>
-      <c r="H283" s="2"/>
-      <c r="I283" s="2"/>
-      <c r="J283" s="2"/>
-      <c r="K283" s="2"/>
-      <c r="L283" s="2"/>
-      <c r="M283" s="2"/>
-      <c r="N283" s="2"/>
-      <c r="O283" s="2"/>
-      <c r="P283" s="2"/>
-      <c r="Q283" s="2"/>
-      <c r="R283" s="2"/>
-      <c r="S283" s="2"/>
-      <c r="T283" s="2"/>
-      <c r="U283" s="2"/>
-      <c r="V283" s="2"/>
-      <c r="W283" s="2"/>
-      <c r="X283" s="2"/>
-      <c r="Y283" s="2"/>
-      <c r="Z283" s="2"/>
-      <c r="AA283" s="2"/>
-      <c r="AB283" s="2"/>
-      <c r="AC283" s="2"/>
-      <c r="AD283" s="2"/>
-      <c r="AE283" s="2"/>
-      <c r="AF283" s="2"/>
-      <c r="AG283" s="2"/>
-      <c r="AH283" s="2"/>
-      <c r="AI283" s="2"/>
-      <c r="AJ283" s="2"/>
-      <c r="AK283" s="2"/>
-      <c r="AL283" s="2"/>
-      <c r="AM283" s="2"/>
-      <c r="AN283" s="2"/>
-      <c r="AO283" s="2"/>
-      <c r="AP283" s="2"/>
-      <c r="AQ283" s="2"/>
-      <c r="AR283" s="2"/>
-      <c r="AS283" s="2"/>
-      <c r="AT283" s="2"/>
-      <c r="AU283" s="2"/>
-      <c r="AV283" s="2"/>
-      <c r="AW283" s="2"/>
-      <c r="AX283" s="2"/>
-      <c r="AY283" s="2"/>
-      <c r="AZ283" s="2"/>
-      <c r="BA283" s="2"/>
-      <c r="BB283" s="2"/>
-      <c r="BC283" s="2"/>
-      <c r="BD283" s="2"/>
-      <c r="BE283" s="2"/>
-      <c r="BF283" s="2"/>
-      <c r="BG283" s="2"/>
-      <c r="BH283" s="2"/>
-      <c r="BI283" s="3"/>
-      <c r="BJ283" s="2"/>
-      <c r="BK283" s="2"/>
-      <c r="BL283" s="2"/>
-      <c r="BM283" s="2"/>
-      <c r="BN283" s="2"/>
-      <c r="BO283" s="2"/>
-      <c r="BP283" s="2"/>
-      <c r="BQ283" s="2"/>
-      <c r="BR283" s="2"/>
-      <c r="BS283" s="2"/>
-      <c r="BT283" s="2"/>
-      <c r="BU283" s="2"/>
-      <c r="BV283" s="2"/>
-      <c r="BW283" s="2"/>
-      <c r="BX283" s="2"/>
-      <c r="BY283" s="2"/>
-      <c r="BZ283" s="2"/>
-      <c r="CA283" s="2"/>
-      <c r="CB283" s="2"/>
-      <c r="CC283" s="2"/>
-      <c r="CD283" s="2"/>
-      <c r="CE283" s="2"/>
-      <c r="CF283" s="2"/>
-      <c r="CG283" s="2"/>
-    </row>
-    <row customFormat="1" r="284" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A284" s="2"/>
-      <c r="B284" s="2"/>
-      <c r="C284" s="3"/>
-      <c r="D284" s="2"/>
-      <c r="E284" s="2"/>
-      <c r="F284" s="2"/>
-      <c r="G284" s="2"/>
-      <c r="H284" s="2"/>
-      <c r="I284" s="2"/>
-      <c r="J284" s="2"/>
-      <c r="K284" s="2"/>
-      <c r="L284" s="2"/>
-      <c r="M284" s="2"/>
-      <c r="N284" s="2"/>
-      <c r="O284" s="2"/>
-      <c r="P284" s="2"/>
-      <c r="Q284" s="2"/>
-      <c r="R284" s="2"/>
-      <c r="S284" s="2"/>
-      <c r="T284" s="2"/>
-      <c r="U284" s="2"/>
-      <c r="V284" s="2"/>
-      <c r="W284" s="2"/>
-      <c r="X284" s="2"/>
-      <c r="Y284" s="2"/>
-      <c r="Z284" s="2"/>
-      <c r="AA284" s="2"/>
-      <c r="AB284" s="2"/>
-      <c r="AC284" s="2"/>
-      <c r="AD284" s="2"/>
-      <c r="AE284" s="2"/>
-      <c r="AF284" s="2"/>
-      <c r="AG284" s="2"/>
-      <c r="AH284" s="2"/>
-      <c r="AI284" s="2"/>
-      <c r="AJ284" s="2"/>
-      <c r="AK284" s="2"/>
-      <c r="AL284" s="2"/>
-      <c r="AM284" s="2"/>
-      <c r="AN284" s="2"/>
-      <c r="AO284" s="2"/>
-      <c r="AP284" s="2"/>
-      <c r="AQ284" s="2"/>
-      <c r="AR284" s="2"/>
-      <c r="AS284" s="2"/>
-      <c r="AT284" s="2"/>
-      <c r="AU284" s="2"/>
-      <c r="AV284" s="2"/>
-      <c r="AW284" s="2"/>
-      <c r="AX284" s="2"/>
-      <c r="AY284" s="2"/>
-      <c r="AZ284" s="2"/>
-      <c r="BA284" s="2"/>
-      <c r="BB284" s="2"/>
-      <c r="BC284" s="2"/>
-      <c r="BD284" s="2"/>
-      <c r="BE284" s="2"/>
-      <c r="BF284" s="2"/>
-      <c r="BG284" s="2"/>
-      <c r="BH284" s="2"/>
-      <c r="BI284" s="3"/>
-      <c r="BJ284" s="2"/>
-      <c r="BK284" s="2"/>
-      <c r="BL284" s="2"/>
-      <c r="BM284" s="2"/>
-      <c r="BN284" s="2"/>
-      <c r="BO284" s="2"/>
-      <c r="BP284" s="2"/>
-      <c r="BQ284" s="2"/>
-      <c r="BR284" s="2"/>
-      <c r="BS284" s="2"/>
-      <c r="BT284" s="2"/>
-      <c r="BU284" s="2"/>
-      <c r="BV284" s="2"/>
-      <c r="BW284" s="2"/>
-      <c r="BX284" s="2"/>
-      <c r="BY284" s="2"/>
-      <c r="BZ284" s="2"/>
-      <c r="CA284" s="2"/>
-      <c r="CB284" s="2"/>
-      <c r="CC284" s="2"/>
-      <c r="CD284" s="2"/>
-      <c r="CE284" s="2"/>
-      <c r="CF284" s="2"/>
-      <c r="CG284" s="2"/>
+      <c r="C283" s="14"/>
+      <c r="BI283" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -30987,7 +30750,7 @@
     <hyperlink r:id="rId18" ref="C73"/>
     <hyperlink r:id="rId19" ref="C25"/>
     <hyperlink r:id="rId20" ref="C11"/>
-    <hyperlink r:id="rId21" ref="C166"/>
+    <hyperlink r:id="rId21" ref="C164"/>
     <hyperlink r:id="rId22" ref="C79"/>
     <hyperlink display="Ankit@12345" r:id="rId23" ref="AU79"/>
     <hyperlink r:id="rId24" ref="C77"/>
@@ -30999,35 +30762,36 @@
     <hyperlink r:id="rId30" ref="C96"/>
     <hyperlink r:id="rId31" ref="C92"/>
     <hyperlink r:id="rId32" ref="C95"/>
-    <hyperlink r:id="rId33" ref="C146"/>
-    <hyperlink display="Deepika@1234" r:id="rId34" ref="D146"/>
-    <hyperlink r:id="rId35" ref="C158"/>
-    <hyperlink r:id="rId36" ref="C159"/>
-    <hyperlink r:id="rId37" ref="C160"/>
-    <hyperlink r:id="rId38" ref="C161"/>
-    <hyperlink r:id="rId39" ref="C163"/>
-    <hyperlink r:id="rId40" ref="C170"/>
-    <hyperlink r:id="rId41" ref="C172"/>
-    <hyperlink r:id="rId42" ref="C173"/>
-    <hyperlink r:id="rId43" ref="D172"/>
-    <hyperlink r:id="rId44" ref="D173"/>
+    <hyperlink r:id="rId33" ref="C145"/>
+    <hyperlink display="Deepika@1234" r:id="rId34" ref="D145"/>
+    <hyperlink r:id="rId35" ref="C156"/>
+    <hyperlink r:id="rId36" ref="C157"/>
+    <hyperlink r:id="rId37" ref="C158"/>
+    <hyperlink r:id="rId38" ref="C159"/>
+    <hyperlink r:id="rId39" ref="C161"/>
+    <hyperlink r:id="rId40" ref="C168"/>
+    <hyperlink r:id="rId41" ref="C170"/>
+    <hyperlink r:id="rId42" ref="C171"/>
+    <hyperlink r:id="rId43" ref="D170"/>
+    <hyperlink r:id="rId44" ref="D171"/>
     <hyperlink r:id="rId45" ref="C54"/>
-    <hyperlink r:id="rId46" ref="C154"/>
-    <hyperlink r:id="rId47" ref="C155"/>
-    <hyperlink r:id="rId48" ref="C156"/>
-    <hyperlink r:id="rId49" ref="C141"/>
-    <hyperlink r:id="rId50" ref="C142"/>
+    <hyperlink r:id="rId46" ref="C152"/>
+    <hyperlink r:id="rId47" ref="C153"/>
+    <hyperlink r:id="rId48" ref="C154"/>
+    <hyperlink r:id="rId49" ref="C140"/>
+    <hyperlink r:id="rId50" ref="C141"/>
     <hyperlink r:id="rId51" ref="AM131"/>
-    <hyperlink r:id="rId52" ref="C164"/>
-    <hyperlink r:id="rId53" ref="C165"/>
-    <hyperlink r:id="rId54" ref="C167"/>
-    <hyperlink r:id="rId55" ref="C168"/>
-    <hyperlink r:id="rId56" ref="C169"/>
+    <hyperlink r:id="rId52" ref="C162"/>
+    <hyperlink r:id="rId53" ref="C163"/>
+    <hyperlink r:id="rId54" ref="C165"/>
+    <hyperlink r:id="rId55" ref="C166"/>
+    <hyperlink r:id="rId56" ref="C167"/>
     <hyperlink r:id="rId57" ref="C111"/>
     <hyperlink display="Ankit@12345" r:id="rId58" ref="D79"/>
+    <hyperlink r:id="rId59" ref="C136"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId59"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Return and Exchange latest updates
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="5715" windowWidth="12900" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="6585" windowWidth="15360" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="5"/>
     <sheet name="Dependencies" r:id="rId2" sheetId="6"/>
     <sheet name="updates" r:id="rId3" sheetId="7"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="503">
   <si>
     <t>Ankit</t>
   </si>
@@ -1125,9 +1126,6 @@
     <t>fctyhtfvvhrtdfdtytyjtnyuguhku</t>
   </si>
   <si>
-    <t>ewxfregtrxcrgrthhcththj</t>
-  </si>
-  <si>
     <t>cf</t>
   </si>
   <si>
@@ -1404,18 +1402,6 @@
     <t>SS_CheckOut_GuestUser_EmptyField</t>
   </si>
   <si>
-    <t>fcdZAgv@gmail.com</t>
-  </si>
-  <si>
-    <t>ssavfd@gmail.com</t>
-  </si>
-  <si>
-    <t>vcfsxcfdv@gmail.com</t>
-  </si>
-  <si>
-    <t>vcvdzsw@gmail.com</t>
-  </si>
-  <si>
     <t>CLOTHING</t>
   </si>
   <si>
@@ -1449,15 +1435,6 @@
     <t>Relevance,Popular,New,Discount,Price : Low,High</t>
   </si>
   <si>
-    <t>fcSAaqr@gmail.com</t>
-  </si>
-  <si>
-    <t>sdxasdss@gmail.com</t>
-  </si>
-  <si>
-    <t>cdAzsZwqsdSfv@gmail.com</t>
-  </si>
-  <si>
     <t>SS_MyAccount_Verify_Order_Details</t>
   </si>
   <si>
@@ -1525,6 +1502,30 @@
   </si>
   <si>
     <t>SS_MyAccount_Verify_Order_ReviewRating_screen</t>
+  </si>
+  <si>
+    <t>productCategory</t>
+  </si>
+  <si>
+    <t>dwasxzsdcqr@gmail.com</t>
+  </si>
+  <si>
+    <t>zszdsas@gmail.com</t>
+  </si>
+  <si>
+    <t>zxsdcfv@gmail.com</t>
+  </si>
+  <si>
+    <t>sfszss@gmail.com</t>
+  </si>
+  <si>
+    <t>ssaszxsddvfd@gmail.com</t>
+  </si>
+  <si>
+    <t>decsdcszsfddv@gmail.com</t>
+  </si>
+  <si>
+    <t>vcxsdsfzacd@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2151,10 +2152,10 @@
   <dimension ref="A1:CH299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B89" xSplit="1" ySplit="1"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B152" xSplit="1" ySplit="1"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="A101" pane="bottomRight" sqref="A101"/>
+      <selection activeCell="A163" pane="bottomRight" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2187,7 @@
         <v>168</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>369</v>
+        <v>495</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>158</v>
@@ -2608,7 +2609,7 @@
       <c r="CE3" s="1"/>
       <c r="CF3" s="18"/>
       <c r="CG3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:85" x14ac:dyDescent="0.25">
@@ -4492,7 +4493,7 @@
       <c r="D24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -4572,7 +4573,7 @@
       <c r="CE24" s="1"/>
       <c r="CF24" s="18"/>
       <c r="CG24" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row ht="45" r="25" spans="1:85" x14ac:dyDescent="0.25">
@@ -4583,7 +4584,7 @@
         <v>365</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>479</v>
+        <v>498</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -5053,7 +5054,7 @@
       <c r="CE29" s="1"/>
       <c r="CF29" s="18"/>
       <c r="CG29" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row ht="45" r="30" spans="1:85" x14ac:dyDescent="0.25">
@@ -5074,7 +5075,7 @@
         <v>59</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -5152,7 +5153,7 @@
       <c r="CE30" s="1"/>
       <c r="CF30" s="18"/>
       <c r="CG30" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="31" spans="1:85" x14ac:dyDescent="0.25">
@@ -5358,7 +5359,7 @@
       <c r="CE32" s="1"/>
       <c r="CF32" s="18"/>
       <c r="CG32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="33" spans="1:85" x14ac:dyDescent="0.25">
@@ -5455,7 +5456,7 @@
       <c r="CE33" s="1"/>
       <c r="CF33" s="18"/>
       <c r="CG33" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="1:85" x14ac:dyDescent="0.25">
@@ -5700,7 +5701,7 @@
         <v>6</v>
       </c>
       <c r="AE36" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
@@ -5802,7 +5803,7 @@
         <v>6</v>
       </c>
       <c r="AF37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
@@ -5857,7 +5858,7 @@
       <c r="CE37" s="1"/>
       <c r="CF37" s="18"/>
       <c r="CG37" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="38" spans="1:85" x14ac:dyDescent="0.25">
@@ -5963,7 +5964,7 @@
     </row>
     <row r="39" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>365</v>
@@ -5973,10 +5974,10 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -5999,10 +6000,10 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="AE39" s="1"/>
       <c r="AF39" s="1"/>
@@ -6064,7 +6065,7 @@
     </row>
     <row r="40" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>365</v>
@@ -6074,10 +6075,10 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -6100,10 +6101,10 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="AD40" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="AE40" s="1"/>
       <c r="AF40" s="1"/>
@@ -6354,7 +6355,7 @@
       <c r="CE42" s="1"/>
       <c r="CF42" s="18"/>
       <c r="CG42" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="43" spans="1:85" x14ac:dyDescent="0.25">
@@ -6578,7 +6579,7 @@
         <v>53</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -6601,13 +6602,13 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
       <c r="AC45" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="AD45" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AE45" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AF45" s="1"/>
       <c r="AG45" s="1"/>
@@ -6760,7 +6761,7 @@
       <c r="CE46" s="1"/>
       <c r="CF46" s="18"/>
       <c r="CG46" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="47" spans="1:85" x14ac:dyDescent="0.25">
@@ -6857,7 +6858,7 @@
       <c r="CE47" s="1"/>
       <c r="CF47" s="18"/>
       <c r="CG47" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:85" x14ac:dyDescent="0.25">
@@ -7168,7 +7169,7 @@
         <v>53</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -7269,7 +7270,7 @@
         <v>53</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -7370,7 +7371,7 @@
         <v>53</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -7471,7 +7472,7 @@
         <v>53</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -7570,7 +7571,7 @@
         <v>53</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -7671,7 +7672,7 @@
         <v>53</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -7750,12 +7751,12 @@
       <c r="CE56" s="1"/>
       <c r="CF56" s="18"/>
       <c r="CG56" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="57" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>365</v>
@@ -7768,7 +7769,7 @@
         <v>53</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -7847,7 +7848,7 @@
       <c r="CE57" s="1"/>
       <c r="CF57" s="18"/>
       <c r="CG57" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:85" x14ac:dyDescent="0.25">
@@ -7865,7 +7866,7 @@
         <v>53</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -7966,7 +7967,7 @@
         <v>53</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -8065,7 +8066,7 @@
         <v>53</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -8170,7 +8171,7 @@
         <v>53</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -8269,7 +8270,7 @@
         <v>53</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
@@ -8360,7 +8361,7 @@
       <c r="CE62" s="1"/>
       <c r="CF62" s="18"/>
       <c r="CG62" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="1:85" x14ac:dyDescent="0.25">
@@ -8378,7 +8379,7 @@
         <v>53</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
@@ -8469,7 +8470,7 @@
       <c r="CE63" s="1"/>
       <c r="CF63" s="18"/>
       <c r="CG63" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="64" spans="1:85" x14ac:dyDescent="0.25">
@@ -8491,7 +8492,7 @@
         <v>53</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -8598,7 +8599,7 @@
         <v>53</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -10150,10 +10151,10 @@
         <v>365</v>
       </c>
       <c r="C81" s="26" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D81" s="27" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -10198,7 +10199,7 @@
       <c r="AS81" s="1"/>
       <c r="AT81" s="1"/>
       <c r="AU81" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AV81" s="1"/>
       <c r="AW81" s="1"/>
@@ -10240,7 +10241,7 @@
       <c r="CE81" s="1"/>
       <c r="CF81" s="1"/>
       <c r="CG81" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="82" spans="1:85" x14ac:dyDescent="0.25">
@@ -11350,19 +11351,19 @@
     </row>
     <row r="93" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D93" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
@@ -11449,19 +11450,19 @@
     </row>
     <row r="94" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D94" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -11548,25 +11549,25 @@
     </row>
     <row ht="30" r="95" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C95" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D95" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
@@ -11630,7 +11631,7 @@
       <c r="BQ95" s="1"/>
       <c r="BR95" s="1"/>
       <c r="BS95" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT95" s="1"/>
       <c r="BU95" s="1"/>
@@ -11646,30 +11647,30 @@
       <c r="CE95" s="1"/>
       <c r="CF95" s="1"/>
       <c r="CG95" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row ht="30" r="96" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D96" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -11733,7 +11734,7 @@
       <c r="BQ96" s="1"/>
       <c r="BR96" s="1"/>
       <c r="BS96" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT96" s="1"/>
       <c r="BU96" s="1"/>
@@ -11754,25 +11755,25 @@
     </row>
     <row ht="30" r="97" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D97" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
@@ -11836,7 +11837,7 @@
       <c r="BQ97" s="1"/>
       <c r="BR97" s="1"/>
       <c r="BS97" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT97" s="1"/>
       <c r="BU97" s="1"/>
@@ -11852,30 +11853,30 @@
       <c r="CE97" s="1"/>
       <c r="CF97" s="1"/>
       <c r="CG97" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row ht="30" r="98" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D98" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
@@ -11939,7 +11940,7 @@
       <c r="BQ98" s="1"/>
       <c r="BR98" s="1"/>
       <c r="BS98" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT98" s="1"/>
       <c r="BU98" s="1"/>
@@ -11960,25 +11961,25 @@
     </row>
     <row ht="30" r="99" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D99" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
@@ -12042,7 +12043,7 @@
       <c r="BQ99" s="1"/>
       <c r="BR99" s="1"/>
       <c r="BS99" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT99" s="1"/>
       <c r="BU99" s="1"/>
@@ -12058,30 +12059,30 @@
       <c r="CE99" s="1"/>
       <c r="CF99" s="1"/>
       <c r="CG99" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row ht="30" r="100" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D100" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
       <c r="I100" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
@@ -12145,7 +12146,7 @@
       <c r="BQ100" s="1"/>
       <c r="BR100" s="1"/>
       <c r="BS100" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT100" s="1"/>
       <c r="BU100" s="1"/>
@@ -12166,25 +12167,25 @@
     </row>
     <row ht="30" r="101" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C101" s="28" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D101" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
@@ -12248,7 +12249,7 @@
       <c r="BQ101" s="1"/>
       <c r="BR101" s="1"/>
       <c r="BS101" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT101" s="1"/>
       <c r="BU101" s="1"/>
@@ -12269,28 +12270,28 @@
     </row>
     <row ht="30" r="102" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D102" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
@@ -12323,16 +12324,16 @@
       <c r="AM102" s="1"/>
       <c r="AN102" s="1"/>
       <c r="AO102" s="1" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="AP102" s="1" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="AQ102" s="1"/>
       <c r="AR102" s="1"/>
       <c r="AS102" s="1"/>
       <c r="AT102" s="1" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="AU102" s="1"/>
       <c r="AV102" s="1"/>
@@ -12342,15 +12343,15 @@
       <c r="AZ102" s="1"/>
       <c r="BA102" s="1"/>
       <c r="BB102" s="1" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="BC102" s="1"/>
       <c r="BD102" s="1" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="BE102" s="1"/>
       <c r="BF102" s="1" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="BG102" s="1"/>
       <c r="BH102" s="1"/>
@@ -12365,7 +12366,7 @@
       <c r="BQ102" s="1"/>
       <c r="BR102" s="1"/>
       <c r="BS102" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT102" s="1"/>
       <c r="BU102" s="1"/>
@@ -12386,25 +12387,25 @@
     </row>
     <row ht="30" r="103" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D103" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
@@ -12468,7 +12469,7 @@
       <c r="BQ103" s="1"/>
       <c r="BR103" s="1"/>
       <c r="BS103" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT103" s="1"/>
       <c r="BU103" s="1"/>
@@ -12489,25 +12490,25 @@
     </row>
     <row ht="30" r="104" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C104" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D104" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
       <c r="I104" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
@@ -12571,7 +12572,7 @@
       <c r="BQ104" s="1"/>
       <c r="BR104" s="1"/>
       <c r="BS104" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT104" s="1"/>
       <c r="BU104" s="1"/>
@@ -12592,25 +12593,25 @@
     </row>
     <row ht="30" r="105" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C105" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D105" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
       <c r="I105" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
@@ -12674,7 +12675,7 @@
       <c r="BQ105" s="1"/>
       <c r="BR105" s="1"/>
       <c r="BS105" s="1" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="BT105" s="1"/>
       <c r="BU105" s="1"/>
@@ -12695,19 +12696,19 @@
     </row>
     <row r="106" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C106" s="28" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D106" s="27" t="s">
         <v>362</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
@@ -13016,7 +13017,7 @@
         <v>28</v>
       </c>
       <c r="K109" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L109" s="1" t="s">
         <v>5</v>
@@ -13129,7 +13130,7 @@
         <v>28</v>
       </c>
       <c r="K110" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>5</v>
@@ -13246,7 +13247,7 @@
         <v>28</v>
       </c>
       <c r="K111" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>5</v>
@@ -13280,13 +13281,13 @@
       <c r="AE111" s="1"/>
       <c r="AF111" s="1"/>
       <c r="AG111" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AH111" s="1" t="s">
         <v>310</v>
       </c>
       <c r="AI111" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AJ111" s="1" t="s">
         <v>29</v>
@@ -13375,7 +13376,7 @@
         <v>28</v>
       </c>
       <c r="K112" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L112" s="1" t="s">
         <v>5</v>
@@ -13490,7 +13491,7 @@
         <v>28</v>
       </c>
       <c r="K113" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L113" s="1" t="s">
         <v>5</v>
@@ -13617,7 +13618,7 @@
         <v>28</v>
       </c>
       <c r="K114" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L114" s="1" t="s">
         <v>5</v>
@@ -13819,7 +13820,7 @@
         <v>365</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -15506,7 +15507,7 @@
     </row>
     <row r="133" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>365</v>
@@ -15520,7 +15521,7 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="2" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="H133" s="3" t="s">
         <v>6</v>
@@ -15860,7 +15861,7 @@
     </row>
     <row r="136" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>365</v>
@@ -15979,7 +15980,7 @@
     </row>
     <row r="137" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>365</v>
@@ -16042,10 +16043,10 @@
       <c r="AL137" s="1"/>
       <c r="AM137" s="1"/>
       <c r="AN137" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO137" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO137" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP137" s="1"/>
       <c r="AQ137" s="1"/>
@@ -16076,12 +16077,12 @@
       <c r="BJ137" s="1"/>
       <c r="BK137" s="1"/>
       <c r="BL137" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM137" s="1"/>
       <c r="BN137" s="1"/>
       <c r="BO137" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP137" s="1"/>
       <c r="BQ137" s="1"/>
@@ -16106,7 +16107,7 @@
     </row>
     <row r="138" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>365</v>
@@ -16169,10 +16170,10 @@
       <c r="AL138" s="1"/>
       <c r="AM138" s="1"/>
       <c r="AN138" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO138" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO138" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP138" s="1"/>
       <c r="AQ138" s="1"/>
@@ -16203,12 +16204,12 @@
       <c r="BJ138" s="1"/>
       <c r="BK138" s="1"/>
       <c r="BL138" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM138" s="1"/>
       <c r="BN138" s="1"/>
       <c r="BO138" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP138" s="1"/>
       <c r="BQ138" s="1"/>
@@ -16233,13 +16234,13 @@
     </row>
     <row r="139" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>362</v>
@@ -16296,10 +16297,10 @@
       <c r="AL139" s="1"/>
       <c r="AM139" s="1"/>
       <c r="AN139" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO139" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO139" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP139" s="1"/>
       <c r="AQ139" s="1"/>
@@ -16330,12 +16331,12 @@
       <c r="BJ139" s="1"/>
       <c r="BK139" s="1"/>
       <c r="BL139" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM139" s="1"/>
       <c r="BN139" s="1"/>
       <c r="BO139" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP139" s="1"/>
       <c r="BQ139" s="1"/>
@@ -16360,13 +16361,13 @@
     </row>
     <row r="140" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>362</v>
@@ -16377,7 +16378,7 @@
         <v>53</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I140" s="1"/>
       <c r="J140" s="2" t="s">
@@ -16423,10 +16424,10 @@
       <c r="AL140" s="1"/>
       <c r="AM140" s="1"/>
       <c r="AN140" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO140" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO140" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP140" s="1"/>
       <c r="AQ140" s="1"/>
@@ -16457,12 +16458,12 @@
       <c r="BJ140" s="1"/>
       <c r="BK140" s="1"/>
       <c r="BL140" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM140" s="1"/>
       <c r="BN140" s="1"/>
       <c r="BO140" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP140" s="1"/>
       <c r="BQ140" s="1"/>
@@ -16487,13 +16488,13 @@
     </row>
     <row r="141" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>362</v>
@@ -16550,10 +16551,10 @@
       <c r="AL141" s="1"/>
       <c r="AM141" s="1"/>
       <c r="AN141" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO141" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO141" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP141" s="1"/>
       <c r="AQ141" s="1"/>
@@ -16584,12 +16585,12 @@
       <c r="BJ141" s="1"/>
       <c r="BK141" s="1"/>
       <c r="BL141" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM141" s="1"/>
       <c r="BN141" s="1"/>
       <c r="BO141" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP141" s="1"/>
       <c r="BQ141" s="1"/>
@@ -16614,13 +16615,13 @@
     </row>
     <row r="142" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>362</v>
@@ -16677,10 +16678,10 @@
       <c r="AL142" s="1"/>
       <c r="AM142" s="1"/>
       <c r="AN142" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO142" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO142" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP142" s="1"/>
       <c r="AQ142" s="1"/>
@@ -16711,12 +16712,12 @@
       <c r="BJ142" s="1"/>
       <c r="BK142" s="1"/>
       <c r="BL142" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM142" s="1"/>
       <c r="BN142" s="1"/>
       <c r="BO142" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP142" s="1"/>
       <c r="BQ142" s="1"/>
@@ -16741,13 +16742,13 @@
     </row>
     <row r="143" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>362</v>
@@ -16804,10 +16805,10 @@
       <c r="AL143" s="1"/>
       <c r="AM143" s="1"/>
       <c r="AN143" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO143" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO143" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP143" s="1"/>
       <c r="AQ143" s="1"/>
@@ -16838,12 +16839,12 @@
       <c r="BJ143" s="1"/>
       <c r="BK143" s="1"/>
       <c r="BL143" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM143" s="1"/>
       <c r="BN143" s="1"/>
       <c r="BO143" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP143" s="1"/>
       <c r="BQ143" s="1"/>
@@ -16868,7 +16869,7 @@
     </row>
     <row r="144" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>365</v>
@@ -16931,10 +16932,10 @@
       <c r="AL144" s="1"/>
       <c r="AM144" s="1"/>
       <c r="AN144" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO144" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO144" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
@@ -16965,12 +16966,12 @@
       <c r="BJ144" s="1"/>
       <c r="BK144" s="1"/>
       <c r="BL144" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM144" s="1"/>
       <c r="BN144" s="1"/>
       <c r="BO144" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP144" s="1"/>
       <c r="BQ144" s="1"/>
@@ -16995,7 +16996,7 @@
     </row>
     <row r="145" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>365</v>
@@ -17058,10 +17059,10 @@
       <c r="AL145" s="1"/>
       <c r="AM145" s="1"/>
       <c r="AN145" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO145" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO145" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP145" s="1"/>
       <c r="AQ145" s="1"/>
@@ -17092,12 +17093,12 @@
       <c r="BJ145" s="1"/>
       <c r="BK145" s="1"/>
       <c r="BL145" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM145" s="1"/>
       <c r="BN145" s="1"/>
       <c r="BO145" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP145" s="1"/>
       <c r="BQ145" s="1"/>
@@ -17122,7 +17123,7 @@
     </row>
     <row r="146" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>365</v>
@@ -17186,10 +17187,10 @@
       <c r="AL146" s="1"/>
       <c r="AM146" s="1"/>
       <c r="AN146" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO146" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO146" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP146" s="1"/>
       <c r="AQ146" s="1"/>
@@ -17220,12 +17221,12 @@
       <c r="BJ146" s="1"/>
       <c r="BK146" s="1"/>
       <c r="BL146" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM146" s="1"/>
       <c r="BN146" s="1"/>
       <c r="BO146" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP146" s="1"/>
       <c r="BQ146" s="1"/>
@@ -17250,7 +17251,7 @@
     </row>
     <row r="147" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>365</v>
@@ -17308,17 +17309,17 @@
       <c r="AG147" s="1"/>
       <c r="AH147" s="1"/>
       <c r="AI147" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AJ147" s="1"/>
       <c r="AK147" s="1"/>
       <c r="AL147" s="1"/>
       <c r="AM147" s="1"/>
       <c r="AN147" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO147" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO147" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP147" s="1"/>
       <c r="AQ147" s="1"/>
@@ -17349,12 +17350,12 @@
       <c r="BJ147" s="1"/>
       <c r="BK147" s="1"/>
       <c r="BL147" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM147" s="1"/>
       <c r="BN147" s="1"/>
       <c r="BO147" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP147" s="1"/>
       <c r="BQ147" s="1"/>
@@ -17379,7 +17380,7 @@
     </row>
     <row r="148" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>365</v>
@@ -17441,13 +17442,13 @@
       <c r="AK148" s="1"/>
       <c r="AL148" s="1"/>
       <c r="AM148" s="26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AN148" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO148" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO148" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP148" s="1"/>
       <c r="AQ148" s="1"/>
@@ -17478,12 +17479,12 @@
       <c r="BJ148" s="1"/>
       <c r="BK148" s="1"/>
       <c r="BL148" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM148" s="1"/>
       <c r="BN148" s="1"/>
       <c r="BO148" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP148" s="1"/>
       <c r="BQ148" s="1"/>
@@ -17508,7 +17509,7 @@
     </row>
     <row r="149" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>365</v>
@@ -17568,15 +17569,15 @@
       <c r="AI149" s="1"/>
       <c r="AJ149" s="1"/>
       <c r="AK149" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AL149" s="1"/>
       <c r="AM149" s="1"/>
       <c r="AN149" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO149" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO149" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP149" s="1"/>
       <c r="AQ149" s="1"/>
@@ -17607,12 +17608,12 @@
       <c r="BJ149" s="1"/>
       <c r="BK149" s="1"/>
       <c r="BL149" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM149" s="1"/>
       <c r="BN149" s="1"/>
       <c r="BO149" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP149" s="1"/>
       <c r="BQ149" s="1"/>
@@ -17637,7 +17638,7 @@
     </row>
     <row r="150" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>365</v>
@@ -17700,10 +17701,10 @@
       <c r="AL150" s="1"/>
       <c r="AM150" s="1"/>
       <c r="AN150" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO150" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO150" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP150" s="1"/>
       <c r="AQ150" s="1"/>
@@ -17734,12 +17735,12 @@
       <c r="BJ150" s="1"/>
       <c r="BK150" s="1"/>
       <c r="BL150" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM150" s="1"/>
       <c r="BN150" s="1"/>
       <c r="BO150" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP150" s="1"/>
       <c r="BQ150" s="1"/>
@@ -17764,7 +17765,7 @@
     </row>
     <row r="151" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>365</v>
@@ -17827,10 +17828,10 @@
       <c r="AL151" s="1"/>
       <c r="AM151" s="1"/>
       <c r="AN151" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO151" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO151" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP151" s="1"/>
       <c r="AQ151" s="1"/>
@@ -17861,12 +17862,12 @@
       <c r="BJ151" s="1"/>
       <c r="BK151" s="1"/>
       <c r="BL151" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM151" s="1"/>
       <c r="BN151" s="1"/>
       <c r="BO151" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP151" s="1"/>
       <c r="BQ151" s="1"/>
@@ -17891,7 +17892,7 @@
     </row>
     <row r="152" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>365</v>
@@ -17954,10 +17955,10 @@
       <c r="AL152" s="1"/>
       <c r="AM152" s="1"/>
       <c r="AN152" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO152" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO152" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP152" s="1"/>
       <c r="AQ152" s="1"/>
@@ -17988,12 +17989,12 @@
       <c r="BJ152" s="1"/>
       <c r="BK152" s="1"/>
       <c r="BL152" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM152" s="1"/>
       <c r="BN152" s="1"/>
       <c r="BO152" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP152" s="1"/>
       <c r="BQ152" s="1"/>
@@ -18018,13 +18019,13 @@
     </row>
     <row r="153" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C153" s="26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>362</v>
@@ -18081,10 +18082,10 @@
       <c r="AL153" s="1"/>
       <c r="AM153" s="1"/>
       <c r="AN153" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO153" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO153" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP153" s="1"/>
       <c r="AQ153" s="1"/>
@@ -18115,12 +18116,12 @@
       <c r="BJ153" s="1"/>
       <c r="BK153" s="1"/>
       <c r="BL153" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM153" s="1"/>
       <c r="BN153" s="1"/>
       <c r="BO153" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP153" s="1"/>
       <c r="BQ153" s="1"/>
@@ -18145,13 +18146,13 @@
     </row>
     <row r="154" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>362</v>
@@ -18208,10 +18209,10 @@
       <c r="AL154" s="1"/>
       <c r="AM154" s="1"/>
       <c r="AN154" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO154" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO154" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP154" s="1"/>
       <c r="AQ154" s="1"/>
@@ -18242,12 +18243,12 @@
       <c r="BJ154" s="1"/>
       <c r="BK154" s="1"/>
       <c r="BL154" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM154" s="1"/>
       <c r="BN154" s="1"/>
       <c r="BO154" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP154" s="1"/>
       <c r="BQ154" s="1"/>
@@ -18272,13 +18273,13 @@
     </row>
     <row r="155" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>362</v>
@@ -18335,10 +18336,10 @@
       <c r="AL155" s="1"/>
       <c r="AM155" s="1"/>
       <c r="AN155" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO155" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO155" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP155" s="1"/>
       <c r="AQ155" s="1"/>
@@ -18369,12 +18370,12 @@
       <c r="BJ155" s="1"/>
       <c r="BK155" s="1"/>
       <c r="BL155" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM155" s="1"/>
       <c r="BN155" s="1"/>
       <c r="BO155" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP155" s="1"/>
       <c r="BQ155" s="1"/>
@@ -18399,13 +18400,13 @@
     </row>
     <row r="156" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>362</v>
@@ -18462,10 +18463,10 @@
       <c r="AL156" s="1"/>
       <c r="AM156" s="1"/>
       <c r="AN156" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO156" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO156" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP156" s="1"/>
       <c r="AQ156" s="1"/>
@@ -18496,12 +18497,12 @@
       <c r="BJ156" s="1"/>
       <c r="BK156" s="1"/>
       <c r="BL156" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM156" s="1"/>
       <c r="BN156" s="1"/>
       <c r="BO156" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP156" s="1"/>
       <c r="BQ156" s="1"/>
@@ -18526,13 +18527,13 @@
     </row>
     <row r="157" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>3</v>
@@ -18589,10 +18590,10 @@
       <c r="AL157" s="1"/>
       <c r="AM157" s="1"/>
       <c r="AN157" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO157" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO157" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
@@ -18623,12 +18624,12 @@
       <c r="BJ157" s="1"/>
       <c r="BK157" s="1"/>
       <c r="BL157" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM157" s="1"/>
       <c r="BN157" s="1"/>
       <c r="BO157" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP157" s="1"/>
       <c r="BQ157" s="1"/>
@@ -18653,13 +18654,13 @@
     </row>
     <row r="158" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>3</v>
@@ -18670,7 +18671,7 @@
         <v>53</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I158" s="1"/>
       <c r="J158" s="2" t="s">
@@ -18716,10 +18717,10 @@
       <c r="AL158" s="1"/>
       <c r="AM158" s="1"/>
       <c r="AN158" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO158" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO158" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP158" s="1"/>
       <c r="AQ158" s="1"/>
@@ -18750,12 +18751,12 @@
       <c r="BJ158" s="1"/>
       <c r="BK158" s="1"/>
       <c r="BL158" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM158" s="1"/>
       <c r="BN158" s="1"/>
       <c r="BO158" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP158" s="1"/>
       <c r="BQ158" s="1"/>
@@ -18780,7 +18781,7 @@
     </row>
     <row r="159" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>365</v>
@@ -18843,10 +18844,10 @@
       <c r="AL159" s="1"/>
       <c r="AM159" s="1"/>
       <c r="AN159" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO159" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO159" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP159" s="1"/>
       <c r="AQ159" s="1"/>
@@ -18877,12 +18878,12 @@
       <c r="BJ159" s="1"/>
       <c r="BK159" s="1"/>
       <c r="BL159" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM159" s="1"/>
       <c r="BN159" s="1"/>
       <c r="BO159" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP159" s="1"/>
       <c r="BQ159" s="1"/>
@@ -18907,7 +18908,7 @@
     </row>
     <row r="160" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>365</v>
@@ -18970,10 +18971,10 @@
       <c r="AL160" s="1"/>
       <c r="AM160" s="1"/>
       <c r="AN160" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AO160" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="AO160" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="AP160" s="1"/>
       <c r="AQ160" s="1"/>
@@ -19004,12 +19005,12 @@
       <c r="BJ160" s="1"/>
       <c r="BK160" s="1"/>
       <c r="BL160" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM160" s="1"/>
       <c r="BN160" s="1"/>
       <c r="BO160" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP160" s="1"/>
       <c r="BQ160" s="1"/>
@@ -19163,7 +19164,7 @@
         <v>365</v>
       </c>
       <c r="C162" s="26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D162" s="26" t="s">
         <v>362</v>
@@ -19288,7 +19289,7 @@
     </row>
     <row r="163" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>365</v>
@@ -19400,7 +19401,7 @@
       <c r="CE163" s="1"/>
       <c r="CF163" s="1"/>
       <c r="CG163" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="164" spans="1:85" x14ac:dyDescent="0.25">
@@ -20004,13 +20005,13 @@
     </row>
     <row r="169" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C169" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>6</v>
@@ -20100,7 +20101,7 @@
       <c r="BM169" s="1"/>
       <c r="BN169" s="1"/>
       <c r="BO169" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP169" s="1"/>
       <c r="BQ169" s="1"/>
@@ -20125,13 +20126,13 @@
     </row>
     <row r="170" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C170" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>6</v>
@@ -20218,12 +20219,12 @@
       <c r="BJ170" s="1"/>
       <c r="BK170" s="1"/>
       <c r="BL170" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM170" s="1"/>
       <c r="BN170" s="1"/>
       <c r="BO170" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="BP170" s="1"/>
       <c r="BQ170" s="1"/>
@@ -20248,13 +20249,13 @@
     </row>
     <row r="171" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>365</v>
       </c>
       <c r="C171" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>6</v>
@@ -20341,7 +20342,7 @@
       <c r="BJ171" s="1"/>
       <c r="BK171" s="1"/>
       <c r="BL171" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BM171" s="1"/>
       <c r="BN171" s="1"/>
@@ -20494,7 +20495,7 @@
         <v>365</v>
       </c>
       <c r="C173" s="26" t="s">
-        <v>462</v>
+        <v>499</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>3</v>
@@ -20626,7 +20627,7 @@
         <v>365</v>
       </c>
       <c r="C174" s="26" t="s">
-        <v>463</v>
+        <v>500</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>3</v>
@@ -20755,7 +20756,7 @@
         <v>365</v>
       </c>
       <c r="C175" s="26" t="s">
-        <v>464</v>
+        <v>501</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>3</v>
@@ -20886,7 +20887,7 @@
         <v>365</v>
       </c>
       <c r="C176" s="26" t="s">
-        <v>465</v>
+        <v>502</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>3</v>
@@ -21099,7 +21100,7 @@
         <v>365</v>
       </c>
       <c r="C178" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D178" s="11" t="s">
         <v>362</v>
@@ -21113,7 +21114,7 @@
         <v>242</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J178" s="1" t="s">
         <v>315</v>
@@ -21235,7 +21236,7 @@
         <v>365</v>
       </c>
       <c r="C179" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D179" s="11" t="s">
         <v>362</v>
@@ -21249,13 +21250,13 @@
         <v>6</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J179" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="K179" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="K179" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="L179" s="1" t="s">
         <v>363</v>
@@ -21297,7 +21298,7 @@
       <c r="AE179" s="1"/>
       <c r="AF179" s="1"/>
       <c r="AG179" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AH179" s="1"/>
       <c r="AI179" s="1"/>
@@ -21360,7 +21361,7 @@
       <c r="CE179" s="1"/>
       <c r="CF179" s="18"/>
       <c r="CG179" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="180" spans="1:85" x14ac:dyDescent="0.25">
@@ -21371,7 +21372,7 @@
         <v>365</v>
       </c>
       <c r="C180" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D180" s="11" t="s">
         <v>362</v>
@@ -21381,7 +21382,7 @@
       <c r="G180" s="3"/>
       <c r="H180" s="1"/>
       <c r="I180" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J180" s="1" t="s">
         <v>315</v>
@@ -21494,7 +21495,7 @@
         <v>365</v>
       </c>
       <c r="C181" s="28" t="s">
-        <v>477</v>
+        <v>496</v>
       </c>
       <c r="D181" s="11" t="s">
         <v>362</v>
@@ -21510,22 +21511,22 @@
         <v>242</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J181" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K181" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="K181" s="2" t="s">
-        <v>375</v>
-      </c>
       <c r="L181" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M181" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="N181" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="N181" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="O181" s="1"/>
       <c r="P181" s="1" t="s">
@@ -21558,7 +21559,7 @@
       <c r="AE181" s="1"/>
       <c r="AF181" s="1"/>
       <c r="AG181" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AH181" s="1"/>
       <c r="AI181" s="1"/>
@@ -21623,7 +21624,7 @@
         <v>365</v>
       </c>
       <c r="C182" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D182" s="11" t="s">
         <v>362</v>
@@ -21637,7 +21638,7 @@
         <v>242</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>315</v>
@@ -21759,7 +21760,7 @@
         <v>365</v>
       </c>
       <c r="C183" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D183" s="11" t="s">
         <v>362</v>
@@ -21769,7 +21770,7 @@
       <c r="G183" s="3"/>
       <c r="H183" s="1"/>
       <c r="I183" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J183" s="1" t="s">
         <v>315</v>
@@ -21891,7 +21892,7 @@
         <v>365</v>
       </c>
       <c r="C184" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D184" s="11" t="s">
         <v>362</v>
@@ -21901,7 +21902,7 @@
       <c r="G184" s="3"/>
       <c r="H184" s="1"/>
       <c r="I184" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J184" s="1" t="s">
         <v>315</v>
@@ -22023,7 +22024,7 @@
         <v>365</v>
       </c>
       <c r="C185" s="28" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
       <c r="D185" s="11" t="s">
         <v>362</v>
@@ -22039,13 +22040,13 @@
         <v>242</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J185" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K185" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="K185" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="L185" s="1" t="s">
         <v>244</v>
@@ -22087,7 +22088,7 @@
       <c r="AE185" s="1"/>
       <c r="AF185" s="1"/>
       <c r="AG185" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AH185" s="1"/>
       <c r="AI185" s="1"/>
@@ -22175,7 +22176,7 @@
         <v>59</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J186" s="1"/>
       <c r="K186" s="2"/>
@@ -22270,7 +22271,7 @@
         <v>285</v>
       </c>
       <c r="D187" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
@@ -22281,7 +22282,7 @@
         <v>59</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J187" s="2" t="s">
         <v>0</v>
@@ -22394,14 +22395,14 @@
         <v>285</v>
       </c>
       <c r="D188" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E188" s="3"/>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
       <c r="I188" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J188" s="2" t="s">
         <v>292</v>
@@ -22503,7 +22504,7 @@
     </row>
     <row ht="30" r="189" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>365</v>
@@ -22579,17 +22580,17 @@
       <c r="AY189" s="1"/>
       <c r="AZ189" s="1"/>
       <c r="BA189" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB189" s="1"/>
       <c r="BC189" s="1"/>
       <c r="BD189" s="1"/>
       <c r="BE189" s="1"/>
       <c r="BF189" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="BG189" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="BG189" s="4" t="s">
-        <v>440</v>
       </c>
       <c r="BH189" s="1"/>
       <c r="BI189" s="1"/>
@@ -22622,7 +22623,7 @@
     </row>
     <row ht="30" r="190" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>365</v>
@@ -22698,17 +22699,17 @@
       <c r="AY190" s="1"/>
       <c r="AZ190" s="1"/>
       <c r="BA190" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB190" s="1"/>
       <c r="BC190" s="1"/>
       <c r="BD190" s="1"/>
       <c r="BE190" s="1"/>
       <c r="BF190" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="BG190" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH190" s="1"/>
       <c r="BI190" s="1"/>
@@ -22741,7 +22742,7 @@
     </row>
     <row ht="30" r="191" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>365</v>
@@ -22817,17 +22818,17 @@
       <c r="AY191" s="1"/>
       <c r="AZ191" s="1"/>
       <c r="BA191" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB191" s="1"/>
       <c r="BC191" s="1"/>
       <c r="BD191" s="1"/>
       <c r="BE191" s="1"/>
       <c r="BF191" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="BG191" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH191" s="1"/>
       <c r="BI191" s="1"/>
@@ -22860,7 +22861,7 @@
     </row>
     <row r="192" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>365</v>
@@ -22936,17 +22937,17 @@
       <c r="AY192" s="1"/>
       <c r="AZ192" s="1"/>
       <c r="BA192" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB192" s="1"/>
       <c r="BC192" s="1"/>
       <c r="BD192" s="1"/>
       <c r="BE192" s="1"/>
       <c r="BF192" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BG192" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH192" s="1"/>
       <c r="BI192" s="1"/>
@@ -22979,7 +22980,7 @@
     </row>
     <row r="193" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>365</v>
@@ -23055,17 +23056,17 @@
       <c r="AY193" s="1"/>
       <c r="AZ193" s="1"/>
       <c r="BA193" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB193" s="1"/>
       <c r="BC193" s="1"/>
       <c r="BD193" s="1"/>
       <c r="BE193" s="1"/>
       <c r="BF193" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BG193" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH193" s="1"/>
       <c r="BI193" s="1"/>
@@ -23098,7 +23099,7 @@
     </row>
     <row r="194" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>365</v>
@@ -23174,17 +23175,17 @@
       <c r="AY194" s="1"/>
       <c r="AZ194" s="1"/>
       <c r="BA194" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB194" s="1"/>
       <c r="BC194" s="1"/>
       <c r="BD194" s="1"/>
       <c r="BE194" s="1"/>
       <c r="BF194" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="BG194" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH194" s="1"/>
       <c r="BI194" s="1"/>
@@ -23217,7 +23218,7 @@
     </row>
     <row ht="30" r="195" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>365</v>
@@ -23291,17 +23292,17 @@
       <c r="AY195" s="1"/>
       <c r="AZ195" s="1"/>
       <c r="BA195" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB195" s="1"/>
       <c r="BC195" s="1"/>
       <c r="BD195" s="1"/>
       <c r="BE195" s="1"/>
       <c r="BF195" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="BG195" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="BG195" s="4" t="s">
-        <v>440</v>
       </c>
       <c r="BH195" s="1"/>
       <c r="BI195" s="1"/>
@@ -23334,7 +23335,7 @@
     </row>
     <row ht="30" r="196" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>365</v>
@@ -23408,17 +23409,17 @@
       <c r="AY196" s="1"/>
       <c r="AZ196" s="1"/>
       <c r="BA196" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB196" s="1"/>
       <c r="BC196" s="1"/>
       <c r="BD196" s="1"/>
       <c r="BE196" s="1"/>
       <c r="BF196" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="BG196" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH196" s="1"/>
       <c r="BI196" s="1"/>
@@ -23451,7 +23452,7 @@
     </row>
     <row ht="30" r="197" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>365</v>
@@ -23525,17 +23526,17 @@
       <c r="AY197" s="1"/>
       <c r="AZ197" s="1"/>
       <c r="BA197" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB197" s="1"/>
       <c r="BC197" s="1"/>
       <c r="BD197" s="1"/>
       <c r="BE197" s="1"/>
       <c r="BF197" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="BG197" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH197" s="1"/>
       <c r="BI197" s="1"/>
@@ -23568,7 +23569,7 @@
     </row>
     <row r="198" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>365</v>
@@ -23642,17 +23643,17 @@
       <c r="AY198" s="1"/>
       <c r="AZ198" s="1"/>
       <c r="BA198" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB198" s="1"/>
       <c r="BC198" s="1"/>
       <c r="BD198" s="1"/>
       <c r="BE198" s="1"/>
       <c r="BF198" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BG198" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH198" s="1"/>
       <c r="BI198" s="1"/>
@@ -23685,7 +23686,7 @@
     </row>
     <row r="199" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>365</v>
@@ -23759,17 +23760,17 @@
       <c r="AY199" s="1"/>
       <c r="AZ199" s="1"/>
       <c r="BA199" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB199" s="1"/>
       <c r="BC199" s="1"/>
       <c r="BD199" s="1"/>
       <c r="BE199" s="1"/>
       <c r="BF199" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BG199" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH199" s="1"/>
       <c r="BI199" s="1"/>
@@ -23802,7 +23803,7 @@
     </row>
     <row r="200" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>365</v>
@@ -23876,17 +23877,17 @@
       <c r="AY200" s="1"/>
       <c r="AZ200" s="1"/>
       <c r="BA200" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB200" s="1"/>
       <c r="BC200" s="1"/>
       <c r="BD200" s="1"/>
       <c r="BE200" s="1"/>
       <c r="BF200" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="BG200" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BH200" s="1"/>
       <c r="BI200" s="1"/>
@@ -23919,7 +23920,7 @@
     </row>
     <row r="201" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>365</v>
@@ -23995,7 +23996,7 @@
       <c r="AY201" s="1"/>
       <c r="AZ201" s="1"/>
       <c r="BA201" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB201" s="1"/>
       <c r="BC201" s="1"/>
@@ -24034,7 +24035,7 @@
     </row>
     <row r="202" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>365</v>
@@ -24108,7 +24109,7 @@
       <c r="AY202" s="1"/>
       <c r="AZ202" s="1"/>
       <c r="BA202" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BB202" s="1"/>
       <c r="BC202" s="1"/>

</xml_diff>